<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@0488faa66560b37433c7e0f4344898171c2572cd 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="151">
   <si>
     <t>Row</t>
   </si>
@@ -169,6 +169,9 @@
     <t>Datasheet</t>
   </si>
   <si>
+    <t>Supplier</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -181,7 +184,7 @@
     <t>C21 C22 C25 C26</t>
   </si>
   <si>
-    <t>2,2nf50v</t>
+    <t>2,2nF50V</t>
   </si>
   <si>
     <t>C_0805_2012Metric</t>
@@ -193,55 +196,73 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>https://www.samsungsem.com/resources/file/global/support/product_catalog/MLCC.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B222KBANNNC/3886829</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>C1 C11 C14 C16 C19 C20 C28 C29 C32</t>
+  </si>
+  <si>
+    <t>100nF25V</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B104KBCNNNC/3886661</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>C13 C17 C18 C23 C24 C27 C30 C31</t>
+  </si>
+  <si>
+    <t>1uF16V</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B105KAFNNNE/3886724</t>
+  </si>
+  <si>
+    <t>C2 C3 C4 C5 C6 C7 C8 C9 C10 C12 C15</t>
+  </si>
+  <si>
+    <t>10uF16V</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21X106KAYNNNE/5961182</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Light emitting diode</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>D1 D2</t>
+  </si>
+  <si>
+    <t>LED_0805_2012Metric</t>
+  </si>
+  <si>
     <t>~</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>C1 C11 C14 C16 C19 C20 C28 C29 C32</t>
-  </si>
-  <si>
-    <t>100nf25v</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>C13 C17 C18 C23 C24 C27 C30 C31</t>
-  </si>
-  <si>
-    <t>1uf16v</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>C2 C3 C4 C5 C6 C7 C8 C9 C10 C12 C15</t>
-  </si>
-  <si>
-    <t>10uf16v</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Light emitting diode</t>
-  </si>
-  <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>D1 D2</t>
-  </si>
-  <si>
-    <t>LED_0805_2012Metric</t>
+    <t/>
   </si>
   <si>
     <t>6</t>
@@ -262,9 +283,6 @@
     <t>7</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>RPi_GPIO</t>
   </si>
   <si>
@@ -292,22 +310,37 @@
     <t>10</t>
   </si>
   <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT100R/1760711</t>
+  </si>
+  <si>
     <t>R16 R17 R18 R19</t>
   </si>
   <si>
     <t>470R</t>
   </si>
   <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT470R/1760300</t>
+  </si>
+  <si>
     <t>R5 R6 R7 R10</t>
   </si>
   <si>
-    <t>3K8</t>
+    <t>3K9</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT3K90/1760599</t>
   </si>
   <si>
     <t>R1 R20 R23 R24 R25</t>
   </si>
   <si>
-    <t>10k</t>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT10K0/1760676</t>
   </si>
   <si>
     <t>12</t>
@@ -319,6 +352,9 @@
     <t>100K</t>
   </si>
   <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FG100K/1712614</t>
+  </si>
+  <si>
     <t>13</t>
   </si>
   <si>
@@ -334,12 +370,33 @@
     <t>SOT-23-5</t>
   </si>
   <si>
-    <t>http://ww1.microchip.com/downloads/en/DeviceDoc/Atmel-8815-SEEPROM-AT24CS01-02-Datasheet.pdf</t>
+    <t>https://ww1.microchip.com/downloads/en/DeviceDoc/AT24C01C-AT24C02C-I2C-Compatible-Two-Wire-Serial-EEPROM-1Kbit-2Kbit-20006111A.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/microchip-technology/AT24C01C-STUM-T/3903763</t>
   </si>
   <si>
     <t>14</t>
   </si>
   <si>
+    <t>TLV71333PDBV-Regulator_Linear</t>
+  </si>
+  <si>
+    <t>U2 U3 U5</t>
+  </si>
+  <si>
+    <t>NCP163</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pub/Collateral/NCP163-D.PDF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/onsemi/NCP163ASN330T1G/9694661</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
     <t>PCM1863DBT-pcm1863</t>
   </si>
   <si>
@@ -355,7 +412,10 @@
     <t>https://www.ti.com/lit/ds/symlink/pcm1863.pdf</t>
   </si>
   <si>
-    <t>15</t>
+    <t>https://www.digikey.ch/de/products/detail/texas-instruments/PCM1863DBT/4895616</t>
+  </si>
+  <si>
+    <t>16</t>
   </si>
   <si>
     <t>PCM5242RHBR-pcm5242</t>
@@ -373,19 +433,7 @@
     <t>https://www.ti.com/lit/ds/symlink/pcm5242.pdf</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>TLV71333PDBV-Regulator_Linear</t>
-  </si>
-  <si>
-    <t>U2 U3 U5</t>
-  </si>
-  <si>
-    <t>ncp163</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pub/Collateral/NCP163-D.PDF</t>
+    <t>https://www.digikey.ch/de/products/detail/texas-instruments/PCM5242RHBR/6571831</t>
   </si>
   <si>
     <t>17</t>
@@ -406,6 +454,9 @@
     <t>https://abracon.com/Oscillators/ASCO.pdf</t>
   </si>
   <si>
+    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ASV-22-5792MHZ-LR-T/15995980</t>
+  </si>
+  <si>
     <t>18</t>
   </si>
   <si>
@@ -415,6 +466,9 @@
     <t>24.576Mhz</t>
   </si>
   <si>
+    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ASDMB-24-576MHZ-LC-T/2809941</t>
+  </si>
+  <si>
     <t>KiBot Bill of Materials</t>
   </si>
   <si>
@@ -493,7 +547,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-23 20:14:36</t>
+    <t>2023-12-26 16:53:53</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -689,12 +743,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8080"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF0FFF4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -708,6 +756,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF0BD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8080"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1268,7 +1322,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1286,11 +1340,12 @@
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
+    <col min="10" max="10" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32" customHeight="1">
+    <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1298,78 +1353,79 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="F2" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="F6" s="3">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -1397,532 +1453,589 @@
       <c r="I8" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" customHeight="1">
+      <c r="A10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1">
+      <c r="A12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="45" customHeight="1">
+      <c r="A14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="5" t="s">
+      <c r="H15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" customHeight="1">
+      <c r="A16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" customHeight="1">
+      <c r="A17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="H17" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="10" t="s">
+      <c r="I17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" customHeight="1">
+      <c r="A18" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30" customHeight="1">
+      <c r="A20" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="45" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="12" t="s">
+      <c r="H21" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="45" customHeight="1">
-      <c r="A14" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="I21" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="9" t="s">
-        <v>65</v>
+        <v>76</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30" customHeight="1">
+      <c r="A22" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="C22" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="9" t="s">
-        <v>77</v>
+        <v>89</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" customHeight="1">
+      <c r="A24" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="C24" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B25" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="9" t="s">
-        <v>88</v>
+        <v>103</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="30" customHeight="1">
+      <c r="A26" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>87</v>
+      <c r="C26" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -1946,7 +2059,7 @@
     <col min="1" max="1" width="37.7109375" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="60.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="61.7109375" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
@@ -1954,7 +2067,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1962,13 +2075,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -1976,13 +2089,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -1991,13 +2104,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G27)</f>
@@ -2006,23 +2119,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2042,27 +2155,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1">
       <c r="A10" s="19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>18</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2073,15 +2189,18 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" ht="30" customHeight="1">
       <c r="A11" s="19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>18</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*9,1)</f>
@@ -2092,15 +2211,18 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="30" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>18</v>
       </c>
       <c r="E12" s="19">
         <f>CEILING(BoardQty*8,1)</f>
@@ -2111,15 +2233,18 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="30" customHeight="1">
       <c r="A13" s="19" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>18</v>
       </c>
       <c r="E13" s="19">
         <f>CEILING(BoardQty*11,1)</f>
@@ -2132,13 +2257,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E14" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2151,13 +2276,13 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="19" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2170,13 +2295,13 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="19" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E16" s="19">
         <f>BoardQty*1</f>
@@ -2189,13 +2314,16 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="19" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>48</v>
+        <v>54</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>56</v>
       </c>
       <c r="E17" s="19">
         <f>CEILING(BoardQty*10,1)</f>
@@ -2208,13 +2336,16 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>48</v>
+        <v>54</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>56</v>
       </c>
       <c r="E18" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2227,13 +2358,16 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>48</v>
+        <v>54</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>56</v>
       </c>
       <c r="E19" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2246,13 +2380,16 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>48</v>
+      <c r="D20" s="19" t="s">
+        <v>56</v>
       </c>
       <c r="E20" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -2265,13 +2402,16 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="19" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>48</v>
+        <v>54</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>56</v>
       </c>
       <c r="E21" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2282,18 +2422,18 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" customHeight="1">
+    <row r="22" spans="1:7" ht="45" customHeight="1">
       <c r="A22" s="19" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="E22" s="19">
         <f>BoardQty*1</f>
@@ -2306,20 +2446,20 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="19" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E23" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*3,1)</f>
+        <v>3</v>
       </c>
       <c r="G23" s="20">
         <f>IF(AND(ISNUMBER(E23),ISNUMBER(F23)),E23*F23,"")</f>
@@ -2328,16 +2468,16 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="19" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -2350,20 +2490,20 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="19" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="E25" s="19">
-        <f>CEILING(BoardQty*3,1)</f>
-        <v>3</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G25" s="20">
         <f>IF(AND(ISNUMBER(E25),ISNUMBER(F25)),E25*F25,"")</f>
@@ -2372,16 +2512,16 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -2394,16 +2534,16 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -2416,15 +2556,15 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="21" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="23" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2523,16 +2663,25 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D22" r:id="rId1"/>
-    <hyperlink ref="D23" r:id="rId2"/>
-    <hyperlink ref="D24" r:id="rId3"/>
-    <hyperlink ref="D25" r:id="rId4"/>
-    <hyperlink ref="D26" r:id="rId5"/>
-    <hyperlink ref="D27" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId1"/>
+    <hyperlink ref="D11" r:id="rId2"/>
+    <hyperlink ref="D12" r:id="rId3"/>
+    <hyperlink ref="D13" r:id="rId4"/>
+    <hyperlink ref="D17" r:id="rId5"/>
+    <hyperlink ref="D18" r:id="rId6"/>
+    <hyperlink ref="D19" r:id="rId7"/>
+    <hyperlink ref="D20" r:id="rId8"/>
+    <hyperlink ref="D21" r:id="rId9"/>
+    <hyperlink ref="D22" r:id="rId10"/>
+    <hyperlink ref="D23" r:id="rId11"/>
+    <hyperlink ref="D24" r:id="rId12"/>
+    <hyperlink ref="D25" r:id="rId13"/>
+    <hyperlink ref="D26" r:id="rId14"/>
+    <hyperlink ref="D27" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId7"/>
-  <legacyDrawing r:id="rId8"/>
+  <drawing r:id="rId16"/>
+  <legacyDrawing r:id="rId17"/>
 </worksheet>
 </file>
 
@@ -2549,72 +2698,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="8" t="s">
-        <v>122</v>
+      <c r="A4" s="11" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@1880acdf820630834144e4f73a6cb894e7d362d5 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="152">
   <si>
     <t>Row</t>
   </si>
@@ -172,6 +172,9 @@
     <t>Supplier</t>
   </si>
   <si>
+    <t>Sim.Enable</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -202,6 +205,9 @@
     <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B222KBANNNC/3886829</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
@@ -262,9 +268,6 @@
     <t>~</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
@@ -547,7 +550,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-27 19:29:13</t>
+    <t>2023-12-27 19:52:58</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -743,6 +746,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF8080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF0FFF4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -756,12 +765,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF0BD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF8080"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1322,7 +1325,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1341,11 +1344,12 @@
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
     <col min="10" max="10" width="60.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32" customHeight="1">
+    <row r="1" spans="1:11" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1354,78 +1358,79 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="C2" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F2" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="C3" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="C4" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+    </row>
+    <row r="5" spans="1:11">
       <c r="C5" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="C6" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F6" s="3">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -1456,586 +1461,643 @@
       <c r="J8" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="30" customHeight="1">
+      <c r="K8" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="30" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="30" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="45" customHeight="1">
+      <c r="A14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="5" t="s">
+      <c r="H15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30" customHeight="1">
+      <c r="A16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30" customHeight="1">
+      <c r="A17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="H17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="30" customHeight="1">
-      <c r="A10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="I17" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30" customHeight="1">
+      <c r="A18" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" customHeight="1">
+      <c r="A20" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="45" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="H21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="10" t="s">
+    </row>
+    <row r="22" spans="1:11" ht="30" customHeight="1">
+      <c r="A22" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="30" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="I22" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="7" t="s">
+      <c r="H23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1">
-      <c r="A12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="I23" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" customHeight="1">
+      <c r="A24" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="10" t="s">
+      <c r="H24" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="45" customHeight="1">
-      <c r="A14" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1">
-      <c r="A16" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="30" customHeight="1">
-      <c r="A18" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="30" customHeight="1">
-      <c r="A19" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="30" customHeight="1">
-      <c r="A20" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="45" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="30" customHeight="1">
-      <c r="A22" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="30" customHeight="1">
-      <c r="A23" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="30" customHeight="1">
-      <c r="A24" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="J24" s="9" t="s">
+      <c r="I24" s="11" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="30" customHeight="1">
+      <c r="J24" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>40</v>
+        <v>99</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D25" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30" customHeight="1">
+      <c r="A26" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="7" t="s">
+      <c r="D26" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="J25" s="6" t="s">
+      <c r="G26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" s="11" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="30" customHeight="1">
-      <c r="A26" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>108</v>
+      <c r="J26" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -2067,7 +2129,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2075,13 +2137,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -2089,13 +2151,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2104,13 +2166,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G27)</f>
@@ -2119,23 +2181,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2155,30 +2217,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
       <c r="A10" s="19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2191,16 +2253,16 @@
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1">
       <c r="A11" s="19" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*9,1)</f>
@@ -2213,16 +2275,16 @@
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" s="19">
         <f>CEILING(BoardQty*8,1)</f>
@@ -2235,16 +2297,16 @@
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1">
       <c r="A13" s="19" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E13" s="19">
         <f>CEILING(BoardQty*11,1)</f>
@@ -2257,13 +2319,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E14" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2276,13 +2338,13 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>43</v>
-      </c>
       <c r="C15" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2295,13 +2357,13 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>47</v>
-      </c>
       <c r="C16" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E16" s="19">
         <f>BoardQty*1</f>
@@ -2314,16 +2376,16 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E17" s="19">
         <f>CEILING(BoardQty*10,1)</f>
@@ -2336,16 +2398,16 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E18" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2358,16 +2420,16 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E19" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2380,16 +2442,16 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E20" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -2402,16 +2464,16 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E21" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2424,16 +2486,16 @@
     </row>
     <row r="22" spans="1:7" ht="45" customHeight="1">
       <c r="A22" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="19" t="s">
-        <v>73</v>
-      </c>
       <c r="C22" s="19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E22" s="19">
         <f>BoardQty*1</f>
@@ -2446,16 +2508,16 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E23" s="19">
         <f>CEILING(BoardQty*3,1)</f>
@@ -2468,16 +2530,16 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -2490,16 +2552,16 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -2512,16 +2574,16 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -2534,16 +2596,16 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -2556,15 +2618,15 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="21" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="23" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2698,72 +2760,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="11" t="s">
-        <v>140</v>
+      <c r="A4" s="8" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@eef4807614ca3b53a2e1f0c4e61958f035bbd554 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -280,7 +280,7 @@
     <t>J2 J3</t>
   </si>
   <si>
-    <t>PinHeader_2x03_P2.54mm_Vertical</t>
+    <t>PinSocket_2x03_P2.54mm_Vertical</t>
   </si>
   <si>
     <t>7</t>
@@ -550,7 +550,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-27 20:46:31</t>
+    <t>2023-12-27 22:08:56</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@0f469fbddc75dd4a029d9494f2b0c59c5803a2b9 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="164">
   <si>
     <t>Row</t>
   </si>
@@ -271,6 +271,30 @@
     <t>6</t>
   </si>
   <si>
+    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>J4 J5</t>
+  </si>
+  <si>
+    <t>Audio_Jack</t>
+  </si>
+  <si>
+    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
@@ -283,7 +307,10 @@
     <t>PinSocket_2x03_P2.54mm_Vertical</t>
   </si>
   <si>
-    <t>7</t>
+    <t>https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=534206&amp;DocType=Customer+Drawing&amp;DocLang=English</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/te-connectivity-amp-connectors/5-534206-3/1093005</t>
   </si>
   <si>
     <t>RPi_GPIO</t>
@@ -295,6 +322,12 @@
     <t>Pin_Header_Straight_2x20</t>
   </si>
   <si>
+    <t>https://cdn-shop.adafruit.com/product-files/2222/00587.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/2222/6238005</t>
+  </si>
+  <si>
     <t>Resistor</t>
   </si>
   <si>
@@ -337,6 +370,9 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT3K90/1760599</t>
   </si>
   <si>
+    <t>12</t>
+  </si>
+  <si>
     <t>R1 R20 R23 R24 R25</t>
   </si>
   <si>
@@ -346,7 +382,7 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT10K0/1760676</t>
   </si>
   <si>
-    <t>12</t>
+    <t>13</t>
   </si>
   <si>
     <t>R4 R9 R11 R13</t>
@@ -358,7 +394,7 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FG100K/1712614</t>
   </si>
   <si>
-    <t>13</t>
+    <t>14</t>
   </si>
   <si>
     <t>I2C Serial EEPROM, 1Kb (128x8) with Unique Serial Number, SOT-23-5</t>
@@ -379,7 +415,7 @@
     <t>https://www.digikey.ch/de/products/detail/microchip-technology/AT24C01C-STUM-T/3903763</t>
   </si>
   <si>
-    <t>14</t>
+    <t>15</t>
   </si>
   <si>
     <t>TLV71333PDBV-Regulator_Linear</t>
@@ -397,7 +433,7 @@
     <t>https://www.digikey.ch/de/products/detail/onsemi/NCP163ASN330T1G/9694661</t>
   </si>
   <si>
-    <t>15</t>
+    <t>16</t>
   </si>
   <si>
     <t>PCM1863DBT-pcm1863</t>
@@ -418,7 +454,7 @@
     <t>https://www.digikey.ch/de/products/detail/texas-instruments/PCM1863DBT/4895616</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
   <si>
     <t>PCM5242RHBR-pcm5242</t>
@@ -439,7 +475,7 @@
     <t>https://www.digikey.ch/de/products/detail/texas-instruments/PCM5242RHBR/6571831</t>
   </si>
   <si>
-    <t>17</t>
+    <t>18</t>
   </si>
   <si>
     <t>ASCO-Oscillator</t>
@@ -460,7 +496,7 @@
     <t>https://www.digikey.ch/de/products/detail/abracon-llc/ASV-22-5792MHZ-LR-T/15995980</t>
   </si>
   <si>
-    <t>18</t>
+    <t>19</t>
   </si>
   <si>
     <t>X2</t>
@@ -511,7 +547,7 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>72 (69 SMD/ 3 THT)</t>
+    <t>74 (69 SMD/ 5 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
@@ -550,7 +586,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-27 23:05:21</t>
+    <t>2023-12-28 20:40:35</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -1325,7 +1361,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1349,7 +1385,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1362,55 +1398,55 @@
     </row>
     <row r="2" spans="1:11">
       <c r="C2" s="2" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="F2" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="C3" s="2" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="C4" s="2" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="C5" s="2" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1418,16 +1454,16 @@
     </row>
     <row r="6" spans="1:11">
       <c r="C6" s="2" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="F6" s="3">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1640,7 +1676,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="45" customHeight="1">
+    <row r="14" spans="1:11" ht="30" customHeight="1">
       <c r="A14" s="9" t="s">
         <v>42</v>
       </c>
@@ -1654,10 +1690,10 @@
         <v>45</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>22</v>
@@ -1665,46 +1701,46 @@
       <c r="H14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>21</v>
+      <c r="I14" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" ht="45" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>21</v>
+        <v>50</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>21</v>
+      <c r="I15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>21</v>
@@ -1714,32 +1750,32 @@
       <c r="A16" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>51</v>
+      <c r="B16" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>18</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K16" s="12" t="s">
         <v>21</v>
@@ -1750,31 +1786,31 @@
         <v>25</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>18</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>21</v>
@@ -1782,22 +1818,22 @@
     </row>
     <row r="18" spans="1:11" ht="30" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>17</v>
@@ -1806,10 +1842,10 @@
         <v>18</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>21</v>
@@ -1820,31 +1856,31 @@
         <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E19" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="G19" s="5" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>18</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>21</v>
@@ -1852,104 +1888,104 @@
     </row>
     <row r="20" spans="1:11" ht="30" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>18</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="K20" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="45" customHeight="1">
+    <row r="21" spans="1:11" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>18</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="30" customHeight="1">
+    <row r="22" spans="1:11" ht="45" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>21</v>
+        <v>84</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>18</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>21</v>
@@ -1957,34 +1993,34 @@
     </row>
     <row r="23" spans="1:11" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E23" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>89</v>
-      </c>
       <c r="G23" s="5" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>18</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>21</v>
@@ -1992,22 +2028,22 @@
     </row>
     <row r="24" spans="1:11" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>11</v>
@@ -2016,10 +2052,10 @@
         <v>18</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="K24" s="12" t="s">
         <v>21</v>
@@ -2027,22 +2063,22 @@
     </row>
     <row r="25" spans="1:11" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>11</v>
@@ -2051,10 +2087,10 @@
         <v>18</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>21</v>
@@ -2062,22 +2098,22 @@
     </row>
     <row r="26" spans="1:11" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>11</v>
@@ -2086,12 +2122,47 @@
         <v>18</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="K26" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="K27" s="8" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2107,7 +2178,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -2129,7 +2200,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2137,13 +2208,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -2151,13 +2222,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2166,38 +2237,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G27)</f>
+        <f>SUM(G10:G28)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2217,16 +2288,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -2341,10 +2412,13 @@
         <v>45</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>48</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2355,19 +2429,22 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" ht="45" customHeight="1">
       <c r="A16" s="19" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="E16" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
       </c>
       <c r="G16" s="20">
         <f>IF(AND(ISNUMBER(E16),ISNUMBER(F16)),E16*F16,"")</f>
@@ -2376,20 +2453,20 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="19" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E17" s="19">
-        <f>CEILING(BoardQty*10,1)</f>
-        <v>10</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G17" s="20">
         <f>IF(AND(ISNUMBER(E17),ISNUMBER(F17)),E17*F17,"")</f>
@@ -2398,20 +2475,20 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E18" s="19">
-        <f>CEILING(BoardQty*4,1)</f>
-        <v>4</v>
+        <f>CEILING(BoardQty*10,1)</f>
+        <v>10</v>
       </c>
       <c r="G18" s="20">
         <f>IF(AND(ISNUMBER(E18),ISNUMBER(F18)),E18*F18,"")</f>
@@ -2420,16 +2497,16 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E19" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2442,20 +2519,20 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="19" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B20" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="19" t="s">
-        <v>55</v>
-      </c>
       <c r="D20" s="19" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E20" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>CEILING(BoardQty*4,1)</f>
+        <v>4</v>
       </c>
       <c r="G20" s="20">
         <f>IF(AND(ISNUMBER(E20),ISNUMBER(F20)),E20*F20,"")</f>
@@ -2464,64 +2541,64 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="19" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E21" s="19">
-        <f>CEILING(BoardQty*4,1)</f>
-        <v>4</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G21" s="20">
         <f>IF(AND(ISNUMBER(E21),ISNUMBER(F21)),E21*F21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45" customHeight="1">
+    <row r="22" spans="1:7">
       <c r="A22" s="19" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E22" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*4,1)</f>
+        <v>4</v>
       </c>
       <c r="G22" s="20">
         <f>IF(AND(ISNUMBER(E22),ISNUMBER(F22)),E22*F22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="45" customHeight="1">
       <c r="A23" s="19" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E23" s="19">
-        <f>CEILING(BoardQty*3,1)</f>
-        <v>3</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G23" s="20">
         <f>IF(AND(ISNUMBER(E23),ISNUMBER(F23)),E23*F23,"")</f>
@@ -2530,20 +2607,20 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="19" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B24" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="19" t="s">
-        <v>89</v>
-      </c>
       <c r="D24" s="19" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E24" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*3,1)</f>
+        <v>3</v>
       </c>
       <c r="G24" s="20">
         <f>IF(AND(ISNUMBER(E24),ISNUMBER(F24)),E24*F24,"")</f>
@@ -2552,16 +2629,16 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="19" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -2574,16 +2651,16 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -2596,16 +2673,16 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -2616,17 +2693,39 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>136</v>
+    <row r="28" spans="1:7">
+      <c r="A28" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G28" s="20">
+        <f>IF(AND(ISNUMBER(E28),ISNUMBER(F28)),E28*F28,"")</f>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="23" t="s">
-        <v>137</v>
+      <c r="A31" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="23" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2724,26 +2823,34 @@
       <formula>AND(ISBLANK(D27),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="expression" dxfId="0" priority="19">
+      <formula>AND(ISBLANK(D28),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
     <hyperlink ref="D12" r:id="rId3"/>
     <hyperlink ref="D13" r:id="rId4"/>
-    <hyperlink ref="D17" r:id="rId5"/>
-    <hyperlink ref="D18" r:id="rId6"/>
-    <hyperlink ref="D19" r:id="rId7"/>
-    <hyperlink ref="D20" r:id="rId8"/>
-    <hyperlink ref="D21" r:id="rId9"/>
-    <hyperlink ref="D22" r:id="rId10"/>
-    <hyperlink ref="D23" r:id="rId11"/>
-    <hyperlink ref="D24" r:id="rId12"/>
-    <hyperlink ref="D25" r:id="rId13"/>
-    <hyperlink ref="D26" r:id="rId14"/>
-    <hyperlink ref="D27" r:id="rId15"/>
+    <hyperlink ref="D15" r:id="rId5"/>
+    <hyperlink ref="D16" r:id="rId6"/>
+    <hyperlink ref="D17" r:id="rId7"/>
+    <hyperlink ref="D18" r:id="rId8"/>
+    <hyperlink ref="D19" r:id="rId9"/>
+    <hyperlink ref="D20" r:id="rId10"/>
+    <hyperlink ref="D21" r:id="rId11"/>
+    <hyperlink ref="D22" r:id="rId12"/>
+    <hyperlink ref="D23" r:id="rId13"/>
+    <hyperlink ref="D24" r:id="rId14"/>
+    <hyperlink ref="D25" r:id="rId15"/>
+    <hyperlink ref="D26" r:id="rId16"/>
+    <hyperlink ref="D27" r:id="rId17"/>
+    <hyperlink ref="D28" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId16"/>
-  <legacyDrawing r:id="rId17"/>
+  <drawing r:id="rId19"/>
+  <legacyDrawing r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -2760,72 +2867,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@8aee33d1b86638a79d6a7e5ddf42295d98a046b5 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -8,13 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="1" r:id="rId1"/>
-    <sheet name="Costs" sheetId="2" r:id="rId2"/>
-    <sheet name="Colors" sheetId="3" r:id="rId3"/>
+    <sheet name="DNF" sheetId="2" r:id="rId2"/>
+    <sheet name="Costs" sheetId="3" r:id="rId3"/>
+    <sheet name="Costs (DNF)" sheetId="4" r:id="rId4"/>
+    <sheet name="Colors" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="BoardQty" localSheetId="1">'Costs'!$G$2</definedName>
+    <definedName name="BoardQty" localSheetId="3">'Costs (DNF)'!$G$2</definedName>
+    <definedName name="BoardQty" localSheetId="2">'Costs'!$G$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BoM!$9:$9</definedName>
-    <definedName name="TotalCost" localSheetId="1">'Costs'!$G$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">DNF!$9:$9</definedName>
+    <definedName name="TotalCost" localSheetId="3">'Costs (DNF)'!$G$4</definedName>
+    <definedName name="TotalCost" localSheetId="2">'Costs'!$G$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -139,8 +144,127 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="F4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Use the minimum extend price across distributors not taking account available quantities.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Schematic identifier for each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Value of each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PCB footprint for each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Manufacturer number for each part and link to it's datasheet (Ctrl-click).
+Purple -&gt; Obsolete part detected by one of the distributors.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Total number of each part needed.
+Gray -&gt; No manf# provided.
+Red -&gt; No parts available.
+Orange -&gt; Not enough parts available.
+Yellow -&gt; Parts available, but haven't purchased enough.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Minimum unit price for each part across all distributors.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Minimum extended price for each part across all distributors.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="165">
   <si>
     <t>Row</t>
   </si>
@@ -271,6 +395,273 @@
     <t>6</t>
   </si>
   <si>
+    <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_02x03_Odd_Even</t>
+  </si>
+  <si>
+    <t>J2 J3</t>
+  </si>
+  <si>
+    <t>PinSocket_2x03_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=534206&amp;DocType=Customer+Drawing&amp;DocLang=English</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/te-connectivity-amp-connectors/5-534206-3/1093005</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>RPi_GPIO</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>Pin_Header_Straight_2x20</t>
+  </si>
+  <si>
+    <t>https://cdn-shop.adafruit.com/product-files/2222/00587.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/2222/6238005</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R2 R3 R8 R12 R14 R15 R21 R22 R26 R27</t>
+  </si>
+  <si>
+    <t>100R</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT100R/1760711</t>
+  </si>
+  <si>
+    <t>R16 R17 R18 R19</t>
+  </si>
+  <si>
+    <t>470R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT470R/1760300</t>
+  </si>
+  <si>
+    <t>R5 R6 R7 R10</t>
+  </si>
+  <si>
+    <t>3K9</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT3K90/1760599</t>
+  </si>
+  <si>
+    <t>R1 R20 R23 R24 R25</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT10K0/1760676</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>R4 R9 R11 R13</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FG100K/1712614</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>I2C Serial EEPROM, 1Kb (128x8) with Unique Serial Number, SOT-23-5</t>
+  </si>
+  <si>
+    <t>AT24CS01-STUM</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>https://ww1.microchip.com/downloads/en/DeviceDoc/AT24C01C-AT24C02C-I2C-Compatible-Two-Wire-Serial-EEPROM-1Kbit-2Kbit-20006111A.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/microchip-technology/AT24C01C-STUM-T/3903763</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>TLV71333PDBV-Regulator_Linear</t>
+  </si>
+  <si>
+    <t>U2 U3 U5</t>
+  </si>
+  <si>
+    <t>NCP163</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pub/Collateral/NCP163-D.PDF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/onsemi/NCP163ASN330T1G/9694661</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>PCM1863DBT-pcm1863</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>PCM1863DBT</t>
+  </si>
+  <si>
+    <t>TSSOP-30_4.4x7.8mm_P0.5mm</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/pcm1863.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/texas-instruments/PCM1863DBT/4895616</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>PCM5242RHBR-pcm5242</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>PCM5242RHBR</t>
+  </si>
+  <si>
+    <t>HVQFN-32-1EP_5x5mm_P0.5mm_EP3.1x3.1mm_ThermalVias</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/pcm5242.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/texas-instruments/PCM5242RHBR/6571831</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>ASCO-Oscillator</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>22.5792Mhz</t>
+  </si>
+  <si>
+    <t>Oscillator_SMD_Abracon_ASDMB-4Pin_2.5x2.0mm</t>
+  </si>
+  <si>
+    <t>https://abracon.com/Oscillators/ASCO.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ASV-22-5792MHZ-LR-T/15995980</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>24.576Mhz</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ASDMB-24-576MHZ-LC-T/2809941</t>
+  </si>
+  <si>
+    <t>KiBot Bill of Materials</t>
+  </si>
+  <si>
+    <t>Schematic:</t>
+  </si>
+  <si>
+    <t>pedalboard-soundcard</t>
+  </si>
+  <si>
+    <t>Variant:</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Revision:</t>
+  </si>
+  <si>
+    <t>0.0.1</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>2023-12-19</t>
+  </si>
+  <si>
+    <t>KiCad Version:</t>
+  </si>
+  <si>
+    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
+  </si>
+  <si>
+    <t>Component Groups:</t>
+  </si>
+  <si>
+    <t>Component Count:</t>
+  </si>
+  <si>
+    <t>74 (69 SMD/ 5 THT)</t>
+  </si>
+  <si>
+    <t>Fitted Components:</t>
+  </si>
+  <si>
+    <t>72 (69 SMD/ 3 THT)</t>
+  </si>
+  <si>
+    <t>Number of PCBs:</t>
+  </si>
+  <si>
+    <t>Total Components:</t>
+  </si>
+  <si>
     <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
   </si>
   <si>
@@ -286,279 +677,15 @@
     <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
   </si>
   <si>
+    <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
     <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
   </si>
   <si>
     <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
-    <t>Conn_02x03_Odd_Even</t>
-  </si>
-  <si>
-    <t>J2 J3</t>
-  </si>
-  <si>
-    <t>PinSocket_2x03_P2.54mm_Vertical</t>
-  </si>
-  <si>
-    <t>https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=534206&amp;DocType=Customer+Drawing&amp;DocLang=English</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/te-connectivity-amp-connectors/5-534206-3/1093005</t>
-  </si>
-  <si>
-    <t>RPi_GPIO</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>Pin_Header_Straight_2x20</t>
-  </si>
-  <si>
-    <t>https://cdn-shop.adafruit.com/product-files/2222/00587.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/2222/6238005</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R2 R3 R8 R12 R14 R15 R21 R22 R26 R27</t>
-  </si>
-  <si>
-    <t>100R</t>
-  </si>
-  <si>
-    <t>R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT100R/1760711</t>
-  </si>
-  <si>
-    <t>R16 R17 R18 R19</t>
-  </si>
-  <si>
-    <t>470R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT470R/1760300</t>
-  </si>
-  <si>
-    <t>R5 R6 R7 R10</t>
-  </si>
-  <si>
-    <t>3K9</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT3K90/1760599</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>R1 R20 R23 R24 R25</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT10K0/1760676</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>R4 R9 R11 R13</t>
-  </si>
-  <si>
-    <t>100K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FG100K/1712614</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>I2C Serial EEPROM, 1Kb (128x8) with Unique Serial Number, SOT-23-5</t>
-  </si>
-  <si>
-    <t>AT24CS01-STUM</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>SOT-23-5</t>
-  </si>
-  <si>
-    <t>https://ww1.microchip.com/downloads/en/DeviceDoc/AT24C01C-AT24C02C-I2C-Compatible-Two-Wire-Serial-EEPROM-1Kbit-2Kbit-20006111A.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/microchip-technology/AT24C01C-STUM-T/3903763</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>TLV71333PDBV-Regulator_Linear</t>
-  </si>
-  <si>
-    <t>U2 U3 U5</t>
-  </si>
-  <si>
-    <t>NCP163</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pub/Collateral/NCP163-D.PDF</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/onsemi/NCP163ASN330T1G/9694661</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>PCM1863DBT-pcm1863</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>PCM1863DBT</t>
-  </si>
-  <si>
-    <t>TSSOP-30_4.4x7.8mm_P0.5mm</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/lit/ds/symlink/pcm1863.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/texas-instruments/PCM1863DBT/4895616</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>PCM5242RHBR-pcm5242</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>PCM5242RHBR</t>
-  </si>
-  <si>
-    <t>HVQFN-32-1EP_5x5mm_P0.5mm_EP3.1x3.1mm_ThermalVias</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/lit/ds/symlink/pcm5242.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/texas-instruments/PCM5242RHBR/6571831</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>ASCO-Oscillator</t>
-  </si>
-  <si>
-    <t>X1</t>
-  </si>
-  <si>
-    <t>22.5792Mhz</t>
-  </si>
-  <si>
-    <t>Oscillator_SMD_Abracon_ASDMB-4Pin_2.5x2.0mm</t>
-  </si>
-  <si>
-    <t>https://abracon.com/Oscillators/ASCO.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ASV-22-5792MHZ-LR-T/15995980</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>X2</t>
-  </si>
-  <si>
-    <t>24.576Mhz</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ASDMB-24-576MHZ-LC-T/2809941</t>
-  </si>
-  <si>
-    <t>KiBot Bill of Materials</t>
-  </si>
-  <si>
-    <t>Schematic:</t>
-  </si>
-  <si>
-    <t>pedalboard-soundcard</t>
-  </si>
-  <si>
-    <t>Variant:</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>Revision:</t>
-  </si>
-  <si>
-    <t>0.0.1</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>2023-12-19</t>
-  </si>
-  <si>
-    <t>KiCad Version:</t>
-  </si>
-  <si>
-    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
-  </si>
-  <si>
-    <t>Component Groups:</t>
-  </si>
-  <si>
-    <t>Component Count:</t>
-  </si>
-  <si>
-    <t>74 (69 SMD/ 5 THT)</t>
-  </si>
-  <si>
-    <t>Fitted Components:</t>
-  </si>
-  <si>
-    <t>Number of PCBs:</t>
-  </si>
-  <si>
-    <t>Total Components:</t>
-  </si>
-  <si>
     <t>Global Part Info</t>
   </si>
   <si>
@@ -586,7 +713,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-28 20:40:35</t>
+    <t>2023-12-28 20:45:35</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
@@ -1034,8 +1161,112 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1464384</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2378784" cy="1285829"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2378784</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2378784" cy="1285829"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>750009</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1361,7 +1592,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1385,7 +1616,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1398,13 +1629,13 @@
     </row>
     <row r="2" spans="1:11">
       <c r="C2" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F2" s="3">
         <v>19</v>
@@ -1412,41 +1643,41 @@
     </row>
     <row r="3" spans="1:11">
       <c r="C3" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="C4" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="C5" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1454,16 +1685,16 @@
     </row>
     <row r="6" spans="1:11">
       <c r="C6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="F6" s="3">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1676,7 +1907,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="30" customHeight="1">
+    <row r="14" spans="1:11" ht="45" customHeight="1">
       <c r="A14" s="9" t="s">
         <v>42</v>
       </c>
@@ -1690,10 +1921,10 @@
         <v>45</v>
       </c>
       <c r="E14" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>22</v>
@@ -1702,45 +1933,45 @@
         <v>18</v>
       </c>
       <c r="I14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="45" customHeight="1">
+    <row r="15" spans="1:11" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="D15" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="E15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="G15" s="5" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>18</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>21</v>
@@ -1750,32 +1981,32 @@
       <c r="A16" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>21</v>
+      <c r="B16" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="C16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="E16" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>57</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>59</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>18</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K16" s="12" t="s">
         <v>21</v>
@@ -1786,31 +2017,31 @@
         <v>25</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>65</v>
-      </c>
       <c r="F17" s="7" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>18</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>21</v>
@@ -1818,22 +2049,22 @@
     </row>
     <row r="18" spans="1:11" ht="30" customHeight="1">
       <c r="A18" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>71</v>
-      </c>
       <c r="F18" s="11" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>17</v>
@@ -1842,10 +2073,10 @@
         <v>18</v>
       </c>
       <c r="I18" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>21</v>
@@ -1856,31 +2087,31 @@
         <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>18</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>21</v>
@@ -1888,104 +2119,104 @@
     </row>
     <row r="20" spans="1:11" ht="30" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>18</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="K20" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30" customHeight="1">
+    <row r="21" spans="1:11" ht="45" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>66</v>
-      </c>
       <c r="G21" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>18</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="45" customHeight="1">
+    <row r="22" spans="1:11" ht="30" customHeight="1">
       <c r="A22" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="D22" s="11" t="s">
         <v>85</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>87</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>86</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>18</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>21</v>
@@ -1993,34 +2224,34 @@
     </row>
     <row r="23" spans="1:11" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>88</v>
-      </c>
       <c r="G23" s="5" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>18</v>
       </c>
       <c r="I23" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J23" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="K23" s="8" t="s">
         <v>21</v>
@@ -2028,22 +2259,22 @@
     </row>
     <row r="24" spans="1:11" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>11</v>
@@ -2052,10 +2283,10 @@
         <v>18</v>
       </c>
       <c r="I24" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="J24" s="10" t="s">
         <v>102</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>103</v>
       </c>
       <c r="K24" s="12" t="s">
         <v>21</v>
@@ -2063,22 +2294,22 @@
     </row>
     <row r="25" spans="1:11" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="F25" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>108</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>11</v>
@@ -2087,10 +2318,10 @@
         <v>18</v>
       </c>
       <c r="I25" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="J25" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>110</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>21</v>
@@ -2098,22 +2329,22 @@
     </row>
     <row r="26" spans="1:11" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>114</v>
-      </c>
       <c r="F26" s="11" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>11</v>
@@ -2122,47 +2353,12 @@
         <v>18</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="30" customHeight="1">
-      <c r="A27" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="K27" s="8" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2178,7 +2374,194 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="60.7109375" customWidth="1"/>
+    <col min="10" max="10" width="60.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="32" customHeight="1">
+      <c r="C1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="C2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="C3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="C4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="C5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="C6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" s="3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -2200,7 +2583,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2208,13 +2591,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -2222,13 +2605,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2237,38 +2620,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G28)</f>
+        <f>SUM(G10:G27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2288,16 +2671,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -2407,18 +2790,18 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" ht="45" customHeight="1">
       <c r="A15" s="19" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="D15" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2429,22 +2812,22 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="45" customHeight="1">
+    <row r="16" spans="1:7">
       <c r="A16" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>55</v>
-      </c>
       <c r="E16" s="19">
-        <f>CEILING(BoardQty*2,1)</f>
-        <v>2</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G16" s="20">
         <f>IF(AND(ISNUMBER(E16),ISNUMBER(F16)),E16*F16,"")</f>
@@ -2453,20 +2836,20 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>58</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>57</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>59</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E17" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*10,1)</f>
+        <v>10</v>
       </c>
       <c r="G17" s="20">
         <f>IF(AND(ISNUMBER(E17),ISNUMBER(F17)),E17*F17,"")</f>
@@ -2475,20 +2858,20 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>65</v>
-      </c>
       <c r="C18" s="19" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E18" s="19">
-        <f>CEILING(BoardQty*10,1)</f>
-        <v>10</v>
+        <f>CEILING(BoardQty*4,1)</f>
+        <v>4</v>
       </c>
       <c r="G18" s="20">
         <f>IF(AND(ISNUMBER(E18),ISNUMBER(F18)),E18*F18,"")</f>
@@ -2497,16 +2880,16 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E19" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2519,20 +2902,20 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E20" s="19">
-        <f>CEILING(BoardQty*4,1)</f>
-        <v>4</v>
+        <f>CEILING(BoardQty*5,1)</f>
+        <v>5</v>
       </c>
       <c r="G20" s="20">
         <f>IF(AND(ISNUMBER(E20),ISNUMBER(F20)),E20*F20,"")</f>
@@ -2541,64 +2924,64 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E21" s="19">
-        <f>CEILING(BoardQty*5,1)</f>
-        <v>5</v>
+        <f>CEILING(BoardQty*4,1)</f>
+        <v>4</v>
       </c>
       <c r="G21" s="20">
         <f>IF(AND(ISNUMBER(E21),ISNUMBER(F21)),E21*F21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" ht="45" customHeight="1">
       <c r="A22" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>68</v>
-      </c>
       <c r="E22" s="19">
-        <f>CEILING(BoardQty*4,1)</f>
-        <v>4</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G22" s="20">
         <f>IF(AND(ISNUMBER(E22),ISNUMBER(F22)),E22*F22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45" customHeight="1">
+    <row r="23" spans="1:7">
       <c r="A23" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>86</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E23" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*3,1)</f>
+        <v>3</v>
       </c>
       <c r="G23" s="20">
         <f>IF(AND(ISNUMBER(E23),ISNUMBER(F23)),E23*F23,"")</f>
@@ -2607,20 +2990,20 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="D24" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>95</v>
-      </c>
       <c r="E24" s="19">
-        <f>CEILING(BoardQty*3,1)</f>
-        <v>3</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G24" s="20">
         <f>IF(AND(ISNUMBER(E24),ISNUMBER(F24)),E24*F24,"")</f>
@@ -2629,16 +3012,16 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="C25" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="D25" s="19" t="s">
         <v>101</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>102</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -2651,16 +3034,16 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="C26" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="D26" s="19" t="s">
         <v>108</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>109</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -2673,16 +3056,16 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -2693,39 +3076,17 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="E28" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
-      </c>
-      <c r="G28" s="20">
-        <f>IF(AND(ISNUMBER(E28),ISNUMBER(F28)),E28*F28,"")</f>
-        <v/>
+    <row r="30" spans="1:7">
+      <c r="A30" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="23" t="s">
-        <v>149</v>
+      <c r="A31" s="23" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2823,11 +3184,6 @@
       <formula>AND(ISBLANK(D27),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28">
-    <cfRule type="expression" dxfId="0" priority="19">
-      <formula>AND(ISBLANK(D28),TRUE())</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
     <hyperlink ref="D11" r:id="rId2"/>
@@ -2846,15 +3202,192 @@
     <hyperlink ref="D25" r:id="rId15"/>
     <hyperlink ref="D26" r:id="rId16"/>
     <hyperlink ref="D27" r:id="rId17"/>
-    <hyperlink ref="D28" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId19"/>
-  <legacyDrawing r:id="rId20"/>
+  <drawing r:id="rId18"/>
+  <legacyDrawing r:id="rId19"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="59.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="32" customHeight="1">
+      <c r="D1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="D2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="D3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G3" s="15">
+        <f>TotalCost/BoardQty</f>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="G4" s="16">
+        <f>SUM(G10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="D5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="19">
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="G10" s="20">
+        <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="23" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="D1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(ISBLANK(D10),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -2867,72 +3400,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@45797088e94bfd3d678359e2b04b959829b5edab 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -428,7 +428,7 @@
     <t>https://cdn-shop.adafruit.com/product-files/2222/00587.pdf</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/2222/6238005</t>
+    <t>https://www.digikey.ch/en/products/detail/adafruit-industries-llc/2222/6238005</t>
   </si>
   <si>
     <t>Resistor</t>
@@ -713,7 +713,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-12-28 20:45:35</t>
+    <t>2023-12-28 21:47:38</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.3</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@16e20904120cd027ee11319bee1124aa5c01cfd9 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -638,7 +638,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
+    <t>7.0.11+1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -713,10 +713,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-01-07 23:01:07</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.18 + KiBot v1.6.3</t>
+    <t>2024-03-12 14:08:07</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.18 + KiBot v1.6.4</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>
@@ -2386,7 +2386,7 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="40.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
@@ -2576,7 +2576,7 @@
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="61.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>
@@ -3226,7 +3226,7 @@
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="59.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@5062527d60d1d7cefc9884fb6fbaf3b1f6e79b11 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="166">
   <si>
     <t>Row</t>
   </si>
@@ -713,10 +713,13 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-03-12 14:08:07</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.18 + KiBot v1.6.4</t>
+    <t>2024-10-04 12:24:52</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.19 + KiBot v1.8.1</t>
+  </si>
+  <si>
+    <t>Columns colors</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>
@@ -731,7 +734,7 @@
     <t>Empty Fields</t>
   </si>
   <si>
-    <t>Costs sheet</t>
+    <t>Costs sheet colors</t>
   </si>
   <si>
     <t>Best price</t>
@@ -3389,83 +3392,88 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5" s="8" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="24" t="s">
+      <c r="A7" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="25" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="27" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="28" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="29" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="31" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="32" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@ef06bb3a7dd2e514dd16f3b134ff966dda655ad9 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="159">
   <si>
     <t>Row</t>
   </si>
@@ -296,13 +296,10 @@
     <t>Supplier</t>
   </si>
   <si>
-    <t>Sim.Enable</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
-    <t>Unpolarized capacitor</t>
+    <t/>
   </si>
   <si>
     <t>C</t>
@@ -329,9 +326,6 @@
     <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B222KBANNNC/3886829</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -377,9 +371,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>Light emitting diode</t>
-  </si>
-  <si>
     <t>LED</t>
   </si>
   <si>
@@ -395,9 +386,6 @@
     <t>6</t>
   </si>
   <si>
-    <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
     <t>Conn_02x03_Odd_Even</t>
   </si>
   <si>
@@ -431,9 +419,6 @@
     <t>https://www.digikey.ch/en/products/detail/adafruit-industries-llc/2222/6238005</t>
   </si>
   <si>
-    <t>Resistor</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -497,9 +482,6 @@
     <t>13</t>
   </si>
   <si>
-    <t>I2C Serial EEPROM, 1Kb (128x8) with Unique Serial Number, SOT-23-5</t>
-  </si>
-  <si>
     <t>AT24CS01-STUM</t>
   </si>
   <si>
@@ -638,7 +620,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>7.0.11+1</t>
+    <t>8.0.4+1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -662,9 +644,6 @@
     <t>Total Components:</t>
   </si>
   <si>
-    <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
-  </si>
-  <si>
     <t>AudioJack3_SwitchTR</t>
   </si>
   <si>
@@ -713,7 +692,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-04 12:24:52</t>
+    <t>2024-10-04 12:56:00</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.1</t>
@@ -900,7 +879,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE6F9FF"/>
+        <fgColor rgb="FFFF8080"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -912,7 +891,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8080"/>
+        <fgColor rgb="FFE6F9FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -924,7 +903,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF0FFFF"/>
+        <fgColor rgb="FFFF8A8A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -936,7 +915,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8A8A"/>
+        <fgColor rgb="FFF0FFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1112,8 +1091,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1464384</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>16584</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1164,8 +1143,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1464384</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>16584</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1595,7 +1574,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1605,7 +1584,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
     <col min="3" max="3" width="34.7109375" customWidth="1"/>
     <col min="4" max="4" width="41.7109375" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" customWidth="1"/>
@@ -1614,12 +1593,11 @@
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
     <col min="10" max="10" width="60.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="32" customHeight="1">
+    <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1628,79 +1606,78 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F2" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F6" s="3">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:10">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -1731,643 +1708,586 @@
       <c r="J8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="4" t="s">
+    </row>
+    <row r="9" spans="1:10" ht="30" customHeight="1">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="30" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="6" t="s">
+    </row>
+    <row r="10" spans="1:10" ht="30" customHeight="1">
+      <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="B10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="30" customHeight="1">
-      <c r="A10" s="9" t="s">
+      <c r="E10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="F10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="11" t="s">
+      <c r="D11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="45" customHeight="1">
+      <c r="A14" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" customHeight="1">
+      <c r="A16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" customHeight="1">
+      <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="11" t="s">
+      <c r="B17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="H17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" customHeight="1">
+      <c r="A18" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30" customHeight="1">
+      <c r="A20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="45" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30" customHeight="1">
+      <c r="A22" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="30" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="30" customHeight="1">
-      <c r="A12" s="9" t="s">
+      <c r="H22" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="45" customHeight="1">
-      <c r="A14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="30" customHeight="1">
-      <c r="A15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="I22" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="30" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="30" customHeight="1">
-      <c r="A16" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="30" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="C23" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="30" customHeight="1">
-      <c r="A18" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" s="9" t="s">
+      <c r="I23" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" customHeight="1">
+      <c r="A24" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="30" customHeight="1">
-      <c r="A19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="30" customHeight="1">
-      <c r="A20" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="9" t="s">
+      <c r="I24" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="30" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J20" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="45" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G21" s="5" t="s">
+      <c r="I25" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="30" customHeight="1">
+      <c r="A26" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="30" customHeight="1">
-      <c r="A22" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="K22" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="30" customHeight="1">
-      <c r="A23" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="30" customHeight="1">
-      <c r="A24" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D24" s="11" t="s">
+      <c r="C26" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="E24" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" s="11" t="s">
+      <c r="D26" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="J24" s="10" t="s">
+      <c r="G26" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="K24" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="30" customHeight="1">
-      <c r="A25" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F25" s="7" t="s">
+      <c r="J26" s="12" t="s">
         <v>107</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="30" customHeight="1">
-      <c r="A26" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="J26" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="K26" s="12" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="C1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -2377,7 +2297,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -2387,7 +2307,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
@@ -2396,12 +2316,11 @@
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
     <col min="10" max="10" width="60.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="32" customHeight="1">
+    <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2410,79 +2329,78 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F2" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F6" s="3">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:10">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -2513,48 +2431,42 @@
       <c r="J8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="4" t="s">
+    </row>
+    <row r="9" spans="1:10" ht="30" customHeight="1">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="30" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="J9" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="C1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -2586,7 +2498,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2594,13 +2506,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -2608,13 +2520,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2623,13 +2535,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G27)</f>
@@ -2638,23 +2550,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2674,30 +2586,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
       <c r="A10" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="C10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>16</v>
-      </c>
       <c r="D10" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2710,16 +2622,16 @@
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1">
       <c r="A11" s="19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" s="19">
         <f>CEILING(BoardQty*9,1)</f>
@@ -2732,16 +2644,16 @@
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="19">
         <f>CEILING(BoardQty*8,1)</f>
@@ -2754,16 +2666,16 @@
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1">
       <c r="A13" s="19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="19">
         <f>CEILING(BoardQty*11,1)</f>
@@ -2776,13 +2688,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E14" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2795,16 +2707,16 @@
     </row>
     <row r="15" spans="1:7" ht="45" customHeight="1">
       <c r="A15" s="19" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2817,16 +2729,16 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E16" s="19">
         <f>BoardQty*1</f>
@@ -2839,16 +2751,16 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="19" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E17" s="19">
         <f>CEILING(BoardQty*10,1)</f>
@@ -2861,16 +2773,16 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E18" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2883,16 +2795,16 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E19" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2905,16 +2817,16 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="19" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E20" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -2927,16 +2839,16 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="19" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E21" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2949,16 +2861,16 @@
     </row>
     <row r="22" spans="1:7" ht="45" customHeight="1">
       <c r="A22" s="19" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E22" s="19">
         <f>BoardQty*1</f>
@@ -2971,16 +2883,16 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="19" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E23" s="19">
         <f>CEILING(BoardQty*3,1)</f>
@@ -2993,16 +2905,16 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="19" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E24" s="19">
         <f>BoardQty*1</f>
@@ -3015,16 +2927,16 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="19" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E25" s="19">
         <f>BoardQty*1</f>
@@ -3037,16 +2949,16 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E26" s="19">
         <f>BoardQty*1</f>
@@ -3059,16 +2971,16 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E27" s="19">
         <f>BoardQty*1</f>
@@ -3081,15 +2993,15 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="21" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="23" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -3236,7 +3148,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3244,13 +3156,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3258,13 +3170,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3273,13 +3185,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10)</f>
@@ -3288,23 +3200,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3324,30 +3236,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3360,15 +3272,15 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="21" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="23" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -3403,77 +3315,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="6" t="s">
-        <v>154</v>
+      <c r="A4" s="8" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="8" t="s">
-        <v>155</v>
+      <c r="A5" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="24" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="26" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="27" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="29" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="30" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="31" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="32" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@1db40af0f6ab3e1fe95bb8dbdb53da2246832402 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="160">
   <si>
     <t>Row</t>
   </si>
@@ -449,7 +449,7 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT470R/1760300</t>
   </si>
   <si>
-    <t>R5 R6 R7 R10</t>
+    <t>R5 R6 R7</t>
   </si>
   <si>
     <t>3K9</t>
@@ -635,7 +635,7 @@
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>72 (69 SMD/ 3 THT)</t>
+    <t>71 (68 SMD/ 3 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -665,6 +665,9 @@
     <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
   </si>
   <si>
+    <t>R10</t>
+  </si>
+  <si>
     <t>Global Part Info</t>
   </si>
   <si>
@@ -692,7 +695,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-04 13:25:20</t>
+    <t>2024-10-14 18:23:31</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.1</t>
@@ -1618,7 +1621,7 @@
         <v>119</v>
       </c>
       <c r="F2" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1674,7 +1677,7 @@
         <v>125</v>
       </c>
       <c r="F6" s="3">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2017,7 +2020,7 @@
         <v>54</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>17</v>
@@ -2297,7 +2300,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -2341,7 +2344,7 @@
         <v>119</v>
       </c>
       <c r="F2" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2397,7 +2400,7 @@
         <v>125</v>
       </c>
       <c r="F6" s="3">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2462,6 +2465,38 @@
       </c>
       <c r="J9" s="8" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2512,7 +2547,7 @@
         <v>110</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -2526,7 +2561,7 @@
         <v>112</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2541,7 +2576,7 @@
         <v>114</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G27)</f>
@@ -2566,7 +2601,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2586,16 +2621,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1">
@@ -2807,8 +2842,8 @@
         <v>56</v>
       </c>
       <c r="E19" s="19">
-        <f>CEILING(BoardQty*4,1)</f>
-        <v>4</v>
+        <f>CEILING(BoardQty*3,1)</f>
+        <v>3</v>
       </c>
       <c r="G19" s="20">
         <f>IF(AND(ISNUMBER(E19),ISNUMBER(F19)),E19*F19,"")</f>
@@ -2993,15 +3028,15 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="21" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3126,7 +3161,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -3162,7 +3197,7 @@
         <v>110</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3176,7 +3211,7 @@
         <v>112</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3191,10 +3226,10 @@
         <v>114</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10)</f>
+        <f>SUM(G10:G11)</f>
         <v>0</v>
       </c>
     </row>
@@ -3216,7 +3251,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3236,16 +3271,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3270,17 +3305,39 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="B13" s="22" t="s">
+    <row r="11" spans="1:7">
+      <c r="A11" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="20">
+        <f>IF(AND(ISNUMBER(E11),ISNUMBER(F11)),E11*F11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="21" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="23" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3293,12 +3350,18 @@
       <formula>AND(ISBLANK(D10),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>AND(ISBLANK(D11),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
+    <hyperlink ref="D11" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -3315,77 +3378,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="24" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="26" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="29" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="30" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="31" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="32" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@734a022232cb1d83cff70071d8b12865fc63a3ab 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -15,11 +15,11 @@
   </sheets>
   <definedNames>
     <definedName name="BoardQty" localSheetId="3">'Costs (DNF)'!$G$2</definedName>
-    <definedName name="BoardQty" localSheetId="2">'Costs'!$G$2</definedName>
+    <definedName name="BoardQty" localSheetId="2">'Costs'!$H$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BoM!$9:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">DNF!$9:$9</definedName>
     <definedName name="TotalCost" localSheetId="3">'Costs (DNF)'!$G$4</definedName>
-    <definedName name="TotalCost" localSheetId="2">'Costs'!$G$4</definedName>
+    <definedName name="TotalCost" localSheetId="2">'Costs'!$H$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -31,7 +31,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="F4" authorId="0">
+    <comment ref="G4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -79,11 +79,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Description of each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>PCB footprint for each part.</t>
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0">
+    <comment ref="E9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0">
+    <comment ref="F9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -114,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0">
+    <comment ref="G9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0">
+    <comment ref="H9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -264,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="165">
   <si>
     <t>Row</t>
   </si>
@@ -329,6 +342,18 @@
     <t>2</t>
   </si>
   <si>
+    <t>C33 C34</t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B104KBCNNNC/3886661</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>C1 C11 C14 C16 C19 C20 C28 C29 C32</t>
   </si>
   <si>
@@ -338,12 +363,6 @@
     <t>9</t>
   </si>
   <si>
-    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B104KBCNNNC/3886661</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>C13 C17 C18 C23 C24 C27 C30 C31</t>
   </si>
   <si>
@@ -356,6 +375,9 @@
     <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B105KAFNNNE/3886724</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>C2 C3 C4 C5 C6 C7 C8 C9 C10 C12 C15</t>
   </si>
   <si>
@@ -368,7 +390,7 @@
     <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21X106KAYNNNE/5961182</t>
   </si>
   <si>
-    <t>5</t>
+    <t>6</t>
   </si>
   <si>
     <t>LED</t>
@@ -383,7 +405,7 @@
     <t>~</t>
   </si>
   <si>
-    <t>6</t>
+    <t>7</t>
   </si>
   <si>
     <t>Conn_02x03_Odd_Even</t>
@@ -401,9 +423,6 @@
     <t>https://www.digikey.ch/de/products/detail/te-connectivity-amp-connectors/5-534206-3/1093005</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>RPi_GPIO</t>
   </si>
   <si>
@@ -458,6 +477,9 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT3K90/1760599</t>
   </si>
   <si>
+    <t>12</t>
+  </si>
+  <si>
     <t>R1 R20 R23 R24 R25</t>
   </si>
   <si>
@@ -467,7 +489,7 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT10K0/1760676</t>
   </si>
   <si>
-    <t>12</t>
+    <t>13</t>
   </si>
   <si>
     <t>R4 R9 R11 R13</t>
@@ -479,7 +501,7 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FG100K/1712614</t>
   </si>
   <si>
-    <t>13</t>
+    <t>14</t>
   </si>
   <si>
     <t>AT24CS01-STUM</t>
@@ -497,10 +519,10 @@
     <t>https://www.digikey.ch/de/products/detail/microchip-technology/AT24C01C-STUM-T/3903763</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>TLV71333PDBV-Regulator_Linear</t>
+    <t>15</t>
+  </si>
+  <si>
+    <t>NCP163ASN330T1G</t>
   </si>
   <si>
     <t>U2 U3 U5</t>
@@ -509,13 +531,13 @@
     <t>NCP163</t>
   </si>
   <si>
-    <t>https://www.onsemi.com/pub/Collateral/NCP163-D.PDF</t>
+    <t>https://www.onsemi.com/pdf/datasheet/ncp163-d.pdf</t>
   </si>
   <si>
     <t>https://www.digikey.ch/de/products/detail/onsemi/NCP163ASN330T1G/9694661</t>
   </si>
   <si>
-    <t>15</t>
+    <t>16</t>
   </si>
   <si>
     <t>PCM1863DBT-pcm1863</t>
@@ -536,7 +558,7 @@
     <t>https://www.digikey.ch/de/products/detail/texas-instruments/PCM1863DBT/4895616</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
   <si>
     <t>PCM5242RHBR-pcm5242</t>
@@ -557,7 +579,7 @@
     <t>https://www.digikey.ch/de/products/detail/texas-instruments/PCM5242RHBR/6571831</t>
   </si>
   <si>
-    <t>17</t>
+    <t>18</t>
   </si>
   <si>
     <t>ASCO-Oscillator</t>
@@ -578,7 +600,7 @@
     <t>https://www.digikey.ch/de/products/detail/abracon-llc/ASV-22-5792MHZ-LR-T/15995980</t>
   </si>
   <si>
-    <t>18</t>
+    <t>19</t>
   </si>
   <si>
     <t>X2</t>
@@ -629,13 +651,13 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>74 (69 SMD/ 5 THT)</t>
+    <t>76 (71 SMD/ 5 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>71 (68 SMD/ 3 THT)</t>
+    <t>73 (70 SMD/ 3 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -683,6 +705,12 @@
     <t>Ext$</t>
   </si>
   <si>
+    <t>Film Capacitor</t>
+  </si>
+  <si>
+    <t>250mA low-noise LDO, 2.2V-5.5V input, 3.3V output, SOT-23-5</t>
+  </si>
+  <si>
     <t>Board Qty:</t>
   </si>
   <si>
@@ -695,7 +723,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-16 11:32:44</t>
+    <t>2024-10-16 13:07:09</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.1</t>
@@ -1577,7 +1605,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1588,7 +1616,7 @@
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="41.7109375" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" customWidth="1"/>
     <col min="6" max="6" width="54.7109375" customWidth="1"/>
@@ -1600,7 +1628,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1612,55 +1640,55 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F2" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1668,16 +1696,16 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F6" s="3">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1764,7 +1792,7 @@
         <v>15</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>17</v>
@@ -1773,12 +1801,12 @@
         <v>18</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>11</v>
@@ -1787,16 +1815,16 @@
         <v>12</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>17</v>
@@ -1805,7 +1833,7 @@
         <v>18</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1">
@@ -1819,16 +1847,16 @@
         <v>12</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>17</v>
@@ -1837,59 +1865,59 @@
         <v>18</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="45" customHeight="1">
+      <c r="I13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>42</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>20</v>
@@ -1897,319 +1925,319 @@
       <c r="H14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="30" customHeight="1">
+      <c r="I14" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="45" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D18" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="11" t="s">
-        <v>62</v>
-      </c>
       <c r="F18" s="11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>65</v>
-      </c>
       <c r="F19" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D20" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="11" t="s">
-        <v>69</v>
-      </c>
       <c r="F20" s="11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J20" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="30" customHeight="1">
+      <c r="A21" s="5" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="45" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>72</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="30" customHeight="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="45" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>10</v>
@@ -2218,30 +2246,30 @@
         <v>17</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>10</v>
@@ -2250,30 +2278,30 @@
         <v>17</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>10</v>
@@ -2282,10 +2310,42 @@
         <v>17</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="J26" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="30" customHeight="1">
+      <c r="A27" s="5" t="s">
         <v>107</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2323,7 +2383,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2335,55 +2395,55 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F2" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2391,16 +2451,16 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F6" s="3">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2443,28 +2503,28 @@
         <v>11</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1">
@@ -2475,28 +2535,28 @@
         <v>11</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2511,11 +2571,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <pane xSplit="8" ySplit="9" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -2524,84 +2584,86 @@
   <cols>
     <col min="1" max="1" width="37.7109375" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="61.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="60.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="50.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="5" max="5" width="61.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32" customHeight="1">
+    <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="G2" s="13">
+        <v>113</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="G3" s="15">
+        <v>115</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
         <v>0.0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="G4" s="16">
-        <f>SUM(G10:G27)</f>
+        <v>117</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="H4" s="16">
+        <f>SUM(H10:H28)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2609,8 +2671,9 @@
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="17"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="18" t="s">
         <v>3</v>
       </c>
@@ -2618,44 +2681,47 @@
         <v>4</v>
       </c>
       <c r="C9" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>135</v>
-      </c>
       <c r="E9" s="18" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1">
+        <v>140</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="D10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="E10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="19">
+      <c r="F10" s="19">
         <f>CEILING(BoardQty*4,1)</f>
         <v>4</v>
       </c>
-      <c r="G10" s="20">
-        <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
+      <c r="H10" s="20">
+        <f>IF(AND(ISNUMBER(F10),ISNUMBER(G10)),F10*G10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1">
+    <row r="11" spans="1:8" ht="30" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>21</v>
       </c>
@@ -2663,499 +2729,533 @@
         <v>22</v>
       </c>
       <c r="C11" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="E11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="19">
+      <c r="F11" s="19">
+        <f>CEILING(BoardQty*2,1)</f>
+        <v>2</v>
+      </c>
+      <c r="H11" s="20">
+        <f>IF(AND(ISNUMBER(F11),ISNUMBER(G11)),F11*G11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" customHeight="1">
+      <c r="A12" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="19">
         <f>CEILING(BoardQty*9,1)</f>
         <v>9</v>
       </c>
-      <c r="G11" s="20">
-        <f>IF(AND(ISNUMBER(E11),ISNUMBER(F11)),E11*F11,"")</f>
+      <c r="H12" s="20">
+        <f>IF(AND(ISNUMBER(F12),ISNUMBER(G12)),F12*G12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" customHeight="1">
-      <c r="A12" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="19" t="s">
+    <row r="13" spans="1:8" ht="30" customHeight="1">
+      <c r="A13" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="E13" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="19">
+      <c r="F13" s="19">
         <f>CEILING(BoardQty*8,1)</f>
         <v>8</v>
       </c>
-      <c r="G12" s="20">
-        <f>IF(AND(ISNUMBER(E12),ISNUMBER(F12)),E12*F12,"")</f>
+      <c r="H13" s="20">
+        <f>IF(AND(ISNUMBER(F13),ISNUMBER(G13)),F13*G13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" customHeight="1">
-      <c r="A13" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="19" t="s">
+    <row r="14" spans="1:8" ht="30" customHeight="1">
+      <c r="A14" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="E14" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="19">
+      <c r="F14" s="19">
         <f>CEILING(BoardQty*11,1)</f>
         <v>11</v>
       </c>
-      <c r="G13" s="20">
-        <f>IF(AND(ISNUMBER(E13),ISNUMBER(F13)),E13*F13,"")</f>
+      <c r="H14" s="20">
+        <f>IF(AND(ISNUMBER(F14),ISNUMBER(G14)),F14*G14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="19">
+    <row r="15" spans="1:8">
+      <c r="A15" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
         <v>2</v>
       </c>
-      <c r="G14" s="20">
-        <f>IF(AND(ISNUMBER(E14),ISNUMBER(F14)),E14*F14,"")</f>
+      <c r="H15" s="20">
+        <f>IF(AND(ISNUMBER(F15),ISNUMBER(G15)),F15*G15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" customHeight="1">
-      <c r="A15" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="19" t="s">
+    <row r="16" spans="1:8" ht="45" customHeight="1">
+      <c r="A16" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="19">
+      <c r="D16" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="19">
         <f>CEILING(BoardQty*2,1)</f>
         <v>2</v>
       </c>
-      <c r="G15" s="20">
-        <f>IF(AND(ISNUMBER(E15),ISNUMBER(F15)),E15*F15,"")</f>
+      <c r="H16" s="20">
+        <f>IF(AND(ISNUMBER(F16),ISNUMBER(G16)),F16*G16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="19" t="s">
+    <row r="17" spans="1:8">
+      <c r="A17" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="19">
+      <c r="D17" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G16" s="20">
-        <f>IF(AND(ISNUMBER(E16),ISNUMBER(F16)),E16*F16,"")</f>
+      <c r="H17" s="20">
+        <f>IF(AND(ISNUMBER(F17),ISNUMBER(G17)),F17*G17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="19" t="s">
+    <row r="18" spans="1:8">
+      <c r="A18" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="B18" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E18" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="19">
         <f>CEILING(BoardQty*10,1)</f>
         <v>10</v>
       </c>
-      <c r="G17" s="20">
-        <f>IF(AND(ISNUMBER(E17),ISNUMBER(F17)),E17*F17,"")</f>
+      <c r="H18" s="20">
+        <f>IF(AND(ISNUMBER(F18),ISNUMBER(G18)),F18*G18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="19" t="s">
+    <row r="19" spans="1:8">
+      <c r="A19" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="19">
+      <c r="F19" s="19">
         <f>CEILING(BoardQty*4,1)</f>
         <v>4</v>
       </c>
-      <c r="G18" s="20">
-        <f>IF(AND(ISNUMBER(E18),ISNUMBER(F18)),E18*F18,"")</f>
+      <c r="H19" s="20">
+        <f>IF(AND(ISNUMBER(F19),ISNUMBER(G19)),F19*G19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="19" t="s">
+    <row r="20" spans="1:8">
+      <c r="A20" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E20" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="19">
         <f>CEILING(BoardQty*3,1)</f>
         <v>3</v>
       </c>
-      <c r="G19" s="20">
-        <f>IF(AND(ISNUMBER(E19),ISNUMBER(F19)),E19*F19,"")</f>
+      <c r="H20" s="20">
+        <f>IF(AND(ISNUMBER(F20),ISNUMBER(G20)),F20*G20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="19" t="s">
+    <row r="21" spans="1:8">
+      <c r="A21" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E21" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="19">
         <f>CEILING(BoardQty*5,1)</f>
         <v>5</v>
       </c>
-      <c r="G20" s="20">
-        <f>IF(AND(ISNUMBER(E20),ISNUMBER(F20)),E20*F20,"")</f>
+      <c r="H21" s="20">
+        <f>IF(AND(ISNUMBER(F21),ISNUMBER(G21)),F21*G21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="19" t="s">
+    <row r="22" spans="1:8">
+      <c r="A22" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E22" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="19">
         <f>CEILING(BoardQty*4,1)</f>
         <v>4</v>
       </c>
-      <c r="G21" s="20">
-        <f>IF(AND(ISNUMBER(E21),ISNUMBER(F21)),E21*F21,"")</f>
+      <c r="H22" s="20">
+        <f>IF(AND(ISNUMBER(F22),ISNUMBER(G22)),F22*G22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45" customHeight="1">
-      <c r="A22" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="19" t="s">
+    <row r="23" spans="1:8" ht="45" customHeight="1">
+      <c r="A23" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="19">
+      <c r="D23" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G22" s="20">
-        <f>IF(AND(ISNUMBER(E22),ISNUMBER(F22)),E22*F22,"")</f>
+      <c r="H23" s="20">
+        <f>IF(AND(ISNUMBER(F23),ISNUMBER(G23)),F23*G23,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" s="19">
+    <row r="24" spans="1:8">
+      <c r="A24" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="19">
         <f>CEILING(BoardQty*3,1)</f>
         <v>3</v>
       </c>
-      <c r="G23" s="20">
-        <f>IF(AND(ISNUMBER(E23),ISNUMBER(F23)),E23*F23,"")</f>
+      <c r="H24" s="20">
+        <f>IF(AND(ISNUMBER(F24),ISNUMBER(G24)),F24*G24,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" s="19" t="s">
+    <row r="25" spans="1:8">
+      <c r="A25" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="19">
+      <c r="B25" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G24" s="20">
-        <f>IF(AND(ISNUMBER(E24),ISNUMBER(F24)),E24*F24,"")</f>
+      <c r="H25" s="20">
+        <f>IF(AND(ISNUMBER(F25),ISNUMBER(G25)),F25*G25,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="19" t="s">
+    <row r="26" spans="1:8">
+      <c r="A26" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="19">
+      <c r="B26" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G25" s="20">
-        <f>IF(AND(ISNUMBER(E25),ISNUMBER(F25)),E25*F25,"")</f>
+      <c r="H26" s="20">
+        <f>IF(AND(ISNUMBER(F26),ISNUMBER(G26)),F26*G26,"")</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="D26" s="19" t="s">
+    <row r="27" spans="1:8">
+      <c r="A27" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="E26" s="19">
+      <c r="B27" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G26" s="20">
-        <f>IF(AND(ISNUMBER(E26),ISNUMBER(F26)),E26*F26,"")</f>
+      <c r="H27" s="20">
+        <f>IF(AND(ISNUMBER(F27),ISNUMBER(G27)),F27*G27,"")</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="19" t="s">
+    <row r="28" spans="1:8">
+      <c r="A28" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27" s="19">
+      <c r="F28" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G27" s="20">
-        <f>IF(AND(ISNUMBER(E27),ISNUMBER(F27)),E27*F27,"")</f>
+      <c r="H28" s="20">
+        <f>IF(AND(ISNUMBER(F28),ISNUMBER(G28)),F28*G28,"")</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="23" t="s">
-        <v>144</v>
+    <row r="31" spans="1:8">
+      <c r="A31" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="23" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="D1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E10">
+  <conditionalFormatting sqref="F10">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(ISBLANK(D10),TRUE())</formula>
+      <formula>AND(ISBLANK(E10),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
+  <conditionalFormatting sqref="F11">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND(ISBLANK(D11),TRUE())</formula>
+      <formula>AND(ISBLANK(E11),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
+  <conditionalFormatting sqref="F12">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>AND(ISBLANK(D12),TRUE())</formula>
+      <formula>AND(ISBLANK(E12),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
+  <conditionalFormatting sqref="F13">
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>AND(ISBLANK(D13),TRUE())</formula>
+      <formula>AND(ISBLANK(E13),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
+  <conditionalFormatting sqref="F14">
     <cfRule type="expression" dxfId="0" priority="5">
-      <formula>AND(ISBLANK(D14),TRUE())</formula>
+      <formula>AND(ISBLANK(E14),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
+  <conditionalFormatting sqref="F15">
     <cfRule type="expression" dxfId="0" priority="6">
-      <formula>AND(ISBLANK(D15),TRUE())</formula>
+      <formula>AND(ISBLANK(E15),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16">
+  <conditionalFormatting sqref="F16">
     <cfRule type="expression" dxfId="0" priority="7">
-      <formula>AND(ISBLANK(D16),TRUE())</formula>
+      <formula>AND(ISBLANK(E16),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
+  <conditionalFormatting sqref="F17">
     <cfRule type="expression" dxfId="0" priority="8">
-      <formula>AND(ISBLANK(D17),TRUE())</formula>
+      <formula>AND(ISBLANK(E17),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
+  <conditionalFormatting sqref="F18">
     <cfRule type="expression" dxfId="0" priority="9">
-      <formula>AND(ISBLANK(D18),TRUE())</formula>
+      <formula>AND(ISBLANK(E18),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
+  <conditionalFormatting sqref="F19">
     <cfRule type="expression" dxfId="0" priority="10">
-      <formula>AND(ISBLANK(D19),TRUE())</formula>
+      <formula>AND(ISBLANK(E19),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E20">
+  <conditionalFormatting sqref="F20">
     <cfRule type="expression" dxfId="0" priority="11">
-      <formula>AND(ISBLANK(D20),TRUE())</formula>
+      <formula>AND(ISBLANK(E20),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
+  <conditionalFormatting sqref="F21">
     <cfRule type="expression" dxfId="0" priority="12">
-      <formula>AND(ISBLANK(D21),TRUE())</formula>
+      <formula>AND(ISBLANK(E21),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
+  <conditionalFormatting sqref="F22">
     <cfRule type="expression" dxfId="0" priority="13">
-      <formula>AND(ISBLANK(D22),TRUE())</formula>
+      <formula>AND(ISBLANK(E22),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
+  <conditionalFormatting sqref="F23">
     <cfRule type="expression" dxfId="0" priority="14">
-      <formula>AND(ISBLANK(D23),TRUE())</formula>
+      <formula>AND(ISBLANK(E23),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
+  <conditionalFormatting sqref="F24">
     <cfRule type="expression" dxfId="0" priority="15">
-      <formula>AND(ISBLANK(D24),TRUE())</formula>
+      <formula>AND(ISBLANK(E24),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
+  <conditionalFormatting sqref="F25">
     <cfRule type="expression" dxfId="0" priority="16">
-      <formula>AND(ISBLANK(D25),TRUE())</formula>
+      <formula>AND(ISBLANK(E25),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E26">
+  <conditionalFormatting sqref="F26">
     <cfRule type="expression" dxfId="0" priority="17">
-      <formula>AND(ISBLANK(D26),TRUE())</formula>
+      <formula>AND(ISBLANK(E26),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
+  <conditionalFormatting sqref="F27">
     <cfRule type="expression" dxfId="0" priority="18">
-      <formula>AND(ISBLANK(D27),TRUE())</formula>
+      <formula>AND(ISBLANK(E27),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28">
+    <cfRule type="expression" dxfId="0" priority="19">
+      <formula>AND(ISBLANK(E28),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1"/>
-    <hyperlink ref="D11" r:id="rId2"/>
-    <hyperlink ref="D12" r:id="rId3"/>
-    <hyperlink ref="D13" r:id="rId4"/>
-    <hyperlink ref="D15" r:id="rId5"/>
-    <hyperlink ref="D16" r:id="rId6"/>
-    <hyperlink ref="D17" r:id="rId7"/>
-    <hyperlink ref="D18" r:id="rId8"/>
-    <hyperlink ref="D19" r:id="rId9"/>
-    <hyperlink ref="D20" r:id="rId10"/>
-    <hyperlink ref="D21" r:id="rId11"/>
-    <hyperlink ref="D22" r:id="rId12"/>
-    <hyperlink ref="D23" r:id="rId13"/>
-    <hyperlink ref="D24" r:id="rId14"/>
-    <hyperlink ref="D25" r:id="rId15"/>
-    <hyperlink ref="D26" r:id="rId16"/>
-    <hyperlink ref="D27" r:id="rId17"/>
+    <hyperlink ref="E10" r:id="rId1"/>
+    <hyperlink ref="E11" r:id="rId2"/>
+    <hyperlink ref="E12" r:id="rId3"/>
+    <hyperlink ref="E13" r:id="rId4"/>
+    <hyperlink ref="E14" r:id="rId5"/>
+    <hyperlink ref="E16" r:id="rId6"/>
+    <hyperlink ref="E17" r:id="rId7"/>
+    <hyperlink ref="E18" r:id="rId8"/>
+    <hyperlink ref="E19" r:id="rId9"/>
+    <hyperlink ref="E20" r:id="rId10"/>
+    <hyperlink ref="E21" r:id="rId11"/>
+    <hyperlink ref="E22" r:id="rId12"/>
+    <hyperlink ref="E23" r:id="rId13"/>
+    <hyperlink ref="E24" r:id="rId14"/>
+    <hyperlink ref="E25" r:id="rId15"/>
+    <hyperlink ref="E26" r:id="rId16"/>
+    <hyperlink ref="E27" r:id="rId17"/>
+    <hyperlink ref="E28" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId18"/>
-  <legacyDrawing r:id="rId19"/>
+  <drawing r:id="rId19"/>
+  <legacyDrawing r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -3183,7 +3283,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3191,13 +3291,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3205,13 +3305,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3220,13 +3320,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G11)</f>
@@ -3235,23 +3335,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3271,30 +3371,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3307,16 +3407,16 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E11" s="19">
         <f>BoardQty*1</f>
@@ -3329,15 +3429,15 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="21" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="23" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -3378,77 +3478,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="24" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="26" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="27" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="29" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="30" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="31" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="32" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@9e9bf81c976ebc61bc46c88f3918851767b93e75 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -630,13 +630,13 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>0.0.1</t>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>Date:</t>
   </si>
   <si>
-    <t>2023-12-19</t>
+    <t>2024-10-16</t>
   </si>
   <si>
     <t>KiCad Version:</t>
@@ -723,7 +723,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-16 16:34:08</t>
+    <t>2024-10-16 16:43:37</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.1</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@695ad573ad28e992da1e594383c4e203e519cfa1 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -630,7 +630,7 @@
     <t>Revision:</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.0.1-RC</t>
   </si>
   <si>
     <t>Date:</t>
@@ -723,7 +723,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-16 16:52:39</t>
+    <t>2024-10-16 20:17:37</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.1</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@d86a8cf2d7602bdbbdcce72082a44764389d3acd 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -277,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="167">
   <si>
     <t>Row</t>
   </si>
@@ -348,21 +348,27 @@
     <t>10nF</t>
   </si>
   <si>
+    <t>https://industrial.panasonic.com/ww/products/pt/film-cap-electroequip/models/ECHU1C103JX5</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/panasonic-electronic-components/ECH-U1C103JX5/353645</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>C1 C11 C14 C16 C19 C20 C28 C29 C32</t>
+  </si>
+  <si>
+    <t>100nF25V</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
     <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B104KBCNNNC/3886661</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>C1 C11 C14 C16 C19 C20 C28 C29 C32</t>
-  </si>
-  <si>
-    <t>100nF25V</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>C13 C17 C18 C23 C24 C27 C30 C31</t>
   </si>
   <si>
@@ -723,7 +729,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-16 20:17:37</t>
+    <t>2024-10-17 10:40:23</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.1</t>
@@ -1628,7 +1634,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1640,13 +1646,13 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F2" s="3">
         <v>21</v>
@@ -1654,41 +1660,41 @@
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1696,13 +1702,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F6" s="3">
         <v>73</v>
@@ -1798,15 +1804,15 @@
         <v>17</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>11</v>
@@ -1815,16 +1821,16 @@
         <v>12</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>17</v>
@@ -1833,7 +1839,7 @@
         <v>18</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1">
@@ -1847,16 +1853,16 @@
         <v>12</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>17</v>
@@ -1865,12 +1871,12 @@
         <v>18</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>11</v>
@@ -1879,16 +1885,16 @@
         <v>12</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>15</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>17</v>
@@ -1897,27 +1903,27 @@
         <v>18</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>20</v>
@@ -1926,7 +1932,7 @@
         <v>17</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J14" s="10" t="s">
         <v>11</v>
@@ -1934,22 +1940,22 @@
     </row>
     <row r="15" spans="1:10" ht="45" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>20</v>
@@ -1958,30 +1964,30 @@
         <v>17</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>10</v>
@@ -1990,62 +1996,62 @@
         <v>17</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>16</v>
@@ -2054,94 +2060,94 @@
         <v>17</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>17</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>16</v>
@@ -2150,30 +2156,30 @@
         <v>17</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="45" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>10</v>
@@ -2182,62 +2188,62 @@
         <v>17</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>10</v>
@@ -2246,30 +2252,30 @@
         <v>17</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>10</v>
@@ -2278,30 +2284,30 @@
         <v>17</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>10</v>
@@ -2310,30 +2316,30 @@
         <v>17</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>10</v>
@@ -2342,10 +2348,10 @@
         <v>17</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2383,7 +2389,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2395,13 +2401,13 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F2" s="3">
         <v>21</v>
@@ -2409,41 +2415,41 @@
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2451,13 +2457,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F6" s="3">
         <v>73</v>
@@ -2503,28 +2509,28 @@
         <v>11</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1">
@@ -2535,28 +2541,28 @@
         <v>11</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2594,7 +2600,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2603,13 +2609,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H2" s="13">
         <v>1</v>
@@ -2617,13 +2623,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2632,13 +2638,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="H4" s="16">
         <f>SUM(H10:H28)</f>
@@ -2647,23 +2653,23 @@
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2687,16 +2693,16 @@
         <v>5</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1">
@@ -2729,13 +2735,13 @@
         <v>22</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2748,10 +2754,10 @@
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>15</v>
@@ -2770,10 +2776,10 @@
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1">
       <c r="A13" s="19" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>15</v>
@@ -2792,10 +2798,10 @@
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1">
       <c r="A14" s="19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>15</v>
@@ -2814,13 +2820,13 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2833,16 +2839,16 @@
     </row>
     <row r="16" spans="1:8" ht="45" customHeight="1">
       <c r="A16" s="19" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F16" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2855,16 +2861,16 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F17" s="19">
         <f>BoardQty*1</f>
@@ -2877,16 +2883,16 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="19" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F18" s="19">
         <f>CEILING(BoardQty*10,1)</f>
@@ -2899,16 +2905,16 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="19" t="s">
         <v>60</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>58</v>
       </c>
       <c r="F19" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2921,16 +2927,16 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F20" s="19">
         <f>CEILING(BoardQty*3,1)</f>
@@ -2943,16 +2949,16 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F21" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -2965,16 +2971,16 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F22" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2987,16 +2993,16 @@
     </row>
     <row r="23" spans="1:8" ht="45" customHeight="1">
       <c r="A23" s="19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F23" s="19">
         <f>BoardQty*1</f>
@@ -3009,19 +3015,19 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="19" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F24" s="19">
         <f>CEILING(BoardQty*3,1)</f>
@@ -3034,16 +3040,16 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="19" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F25" s="19">
         <f>BoardQty*1</f>
@@ -3056,16 +3062,16 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F26" s="19">
         <f>BoardQty*1</f>
@@ -3078,16 +3084,16 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="19" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F27" s="19">
         <f>BoardQty*1</f>
@@ -3100,16 +3106,16 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="19" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F28" s="19">
         <f>BoardQty*1</f>
@@ -3122,15 +3128,15 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="21" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="23" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -3283,7 +3289,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3291,13 +3297,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3305,13 +3311,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3320,13 +3326,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G11)</f>
@@ -3335,23 +3341,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3371,30 +3377,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3407,16 +3413,16 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E11" s="19">
         <f>BoardQty*1</f>
@@ -3429,15 +3435,15 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="21" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="23" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -3478,77 +3484,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="24" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="26" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="27" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="29" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="30" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="31" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="32" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@f453ff3d504841b6952750bd6e648f4d40e042b1 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -277,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="168">
   <si>
     <t>Row</t>
   </si>
@@ -321,7 +321,7 @@
     <t>C21 C22 C25 C26</t>
   </si>
   <si>
-    <t>2,2nF50V</t>
+    <t>2n2</t>
   </si>
   <si>
     <t>C_0805_2012Metric</t>
@@ -345,7 +345,7 @@
     <t>C33 C34</t>
   </si>
   <si>
-    <t>10nF</t>
+    <t>10n_film</t>
   </si>
   <si>
     <t>https://industrial.panasonic.com/ww/products/pt/film-cap-electroequip/models/ECHU1C103JX5</t>
@@ -360,7 +360,7 @@
     <t>C1 C11 C14 C16 C19 C20 C28 C29 C32</t>
   </si>
   <si>
-    <t>100nF25V</t>
+    <t>100n</t>
   </si>
   <si>
     <t>9</t>
@@ -372,7 +372,7 @@
     <t>C13 C17 C18 C23 C24 C27 C30 C31</t>
   </si>
   <si>
-    <t>1uF16V</t>
+    <t>1u</t>
   </si>
   <si>
     <t>8</t>
@@ -387,7 +387,7 @@
     <t>C2 C3 C4 C5 C6 C7 C8 C9 C10 C12 C15</t>
   </si>
   <si>
-    <t>10uF16V</t>
+    <t>10u</t>
   </si>
   <si>
     <t>11</t>
@@ -405,6 +405,9 @@
     <t>D1 D2</t>
   </si>
   <si>
+    <t>red</t>
+  </si>
+  <si>
     <t>LED_0805_2012Metric</t>
   </si>
   <si>
@@ -594,7 +597,7 @@
     <t>X1</t>
   </si>
   <si>
-    <t>22.5792Mhz</t>
+    <t>22.5792M</t>
   </si>
   <si>
     <t>Oscillator_SMD_Abracon_ASDMB-4Pin_2.5x2.0mm</t>
@@ -612,7 +615,7 @@
     <t>X2</t>
   </si>
   <si>
-    <t>24.576Mhz</t>
+    <t>24.576M</t>
   </si>
   <si>
     <t>https://www.digikey.ch/de/products/detail/abracon-llc/ASDMB-24-576MHZ-LC-T/2809941</t>
@@ -648,7 +651,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>8.0.4+1</t>
+    <t>8.0.6+1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -729,10 +732,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-17 10:40:23</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.19 + KiBot v1.8.1</t>
+    <t>2024-12-15 13:25:04</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.19 + KiBot v1.8.2</t>
   </si>
   <si>
     <t>Columns colors</t>
@@ -1128,10 +1131,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>16584</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123779</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>957675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>297815</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1158,7 +1161,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2378784" cy="1285829"/>
+          <a:ext cx="9396825" cy="5079365"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1180,10 +1183,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>16584</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123779</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2691225</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>107315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1210,7 +1213,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2378784" cy="1285829"/>
+          <a:ext cx="9396825" cy="5079365"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1232,10 +1235,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2378784</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123779</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1452975</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>107315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1262,7 +1265,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2378784" cy="1285829"/>
+          <a:ext cx="9396825" cy="5079365"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1284,10 +1287,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>750009</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123779</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1338675</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>107315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1314,7 +1317,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2378784" cy="1285829"/>
+          <a:ext cx="9396825" cy="5079365"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1634,7 +1637,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1646,13 +1649,13 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F2" s="3">
         <v>21</v>
@@ -1660,41 +1663,41 @@
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1702,13 +1705,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F6" s="3">
         <v>73</v>
@@ -1920,10 +1923,10 @@
         <v>41</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>20</v>
@@ -1932,7 +1935,7 @@
         <v>17</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J14" s="10" t="s">
         <v>11</v>
@@ -1940,22 +1943,22 @@
     </row>
     <row r="15" spans="1:10" ht="45" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>45</v>
-      </c>
       <c r="F15" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>20</v>
@@ -1964,10 +1967,10 @@
         <v>17</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
@@ -1978,16 +1981,16 @@
         <v>11</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D16" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="F16" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>10</v>
@@ -1996,10 +1999,10 @@
         <v>17</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1">
@@ -2010,48 +2013,48 @@
         <v>11</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>16</v>
@@ -2060,10 +2063,10 @@
         <v>17</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1">
@@ -2074,16 +2077,16 @@
         <v>11</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>25</v>
@@ -2092,30 +2095,30 @@
         <v>17</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>34</v>
@@ -2124,30 +2127,30 @@
         <v>17</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>16</v>
@@ -2156,30 +2159,30 @@
         <v>17</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="45" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D22" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>77</v>
-      </c>
       <c r="F22" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>10</v>
@@ -2188,30 +2191,30 @@
         <v>17</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>25</v>
@@ -2220,30 +2223,30 @@
         <v>17</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>10</v>
@@ -2252,30 +2255,30 @@
         <v>17</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>10</v>
@@ -2284,30 +2287,30 @@
         <v>17</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>10</v>
@@ -2316,30 +2319,30 @@
         <v>17</v>
       </c>
       <c r="I26" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>10</v>
@@ -2348,10 +2351,10 @@
         <v>17</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2389,7 +2392,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2401,13 +2404,13 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F2" s="3">
         <v>21</v>
@@ -2415,41 +2418,41 @@
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2457,13 +2460,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F6" s="3">
         <v>73</v>
@@ -2509,28 +2512,28 @@
         <v>11</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1">
@@ -2541,28 +2544,28 @@
         <v>11</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2600,7 +2603,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2609,13 +2612,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H2" s="13">
         <v>1</v>
@@ -2623,13 +2626,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2638,13 +2641,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H4" s="16">
         <f>SUM(H10:H28)</f>
@@ -2653,23 +2656,23 @@
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2693,16 +2696,16 @@
         <v>5</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1">
@@ -2735,7 +2738,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>15</v>
@@ -2823,10 +2826,10 @@
         <v>41</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2839,16 +2842,16 @@
     </row>
     <row r="16" spans="1:8" ht="45" customHeight="1">
       <c r="A16" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>45</v>
-      </c>
       <c r="D16" s="19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F16" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2861,16 +2864,16 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>50</v>
-      </c>
       <c r="D17" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F17" s="19">
         <f>BoardQty*1</f>
@@ -2883,16 +2886,16 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F18" s="19">
         <f>CEILING(BoardQty*10,1)</f>
@@ -2905,16 +2908,16 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F19" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2927,16 +2930,16 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F20" s="19">
         <f>CEILING(BoardQty*3,1)</f>
@@ -2949,16 +2952,16 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F21" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -2971,16 +2974,16 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F22" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2993,16 +2996,16 @@
     </row>
     <row r="23" spans="1:8" ht="45" customHeight="1">
       <c r="A23" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>77</v>
-      </c>
       <c r="D23" s="19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F23" s="19">
         <f>BoardQty*1</f>
@@ -3015,19 +3018,19 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F24" s="19">
         <f>CEILING(BoardQty*3,1)</f>
@@ -3040,16 +3043,16 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F25" s="19">
         <f>BoardQty*1</f>
@@ -3062,16 +3065,16 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F26" s="19">
         <f>BoardQty*1</f>
@@ -3084,16 +3087,16 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F27" s="19">
         <f>BoardQty*1</f>
@@ -3106,16 +3109,16 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="19" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F28" s="19">
         <f>BoardQty*1</f>
@@ -3128,15 +3131,15 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="21" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="23" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -3289,7 +3292,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3297,13 +3300,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3311,13 +3314,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3326,13 +3329,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G11)</f>
@@ -3341,23 +3344,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3377,30 +3380,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3413,16 +3416,16 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E11" s="19">
         <f>BoardQty*1</f>
@@ -3435,15 +3438,15 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="21" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="23" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -3484,77 +3487,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="24" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="26" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="27" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="29" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="30" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="31" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="32" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@05a17fdb1a47ef051d8d661718491cc3050219a2 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -405,7 +405,7 @@
     <t>D1 D2</t>
   </si>
   <si>
-    <t>red</t>
+    <t>LED_R</t>
   </si>
   <si>
     <t>LED_0805_2012Metric</t>
@@ -732,7 +732,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-12-15 13:25:04</t>
+    <t>2024-12-15 19:49:32</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.2</t>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@26f3ca50cc2e0b2273ee93242bc51fa4416f000b 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -603,10 +603,10 @@
     <t>Oscillator_SMD_Abracon_ASDMB-4Pin_2.5x2.0mm</t>
   </si>
   <si>
-    <t>https://abracon.com/Oscillators/ASCO.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ASV-22-5792MHZ-LR-T/15995980</t>
+    <t>https://media.digikey.com/pdf/Data%20Sheets/Kyocera%20International/Z_Series_X_Type.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/en/products/detail/kyocera-avx/KC2016Z22-5792C1KX00/11610237</t>
   </si>
   <si>
     <t>19</t>
@@ -618,7 +618,7 @@
     <t>24.576M</t>
   </si>
   <si>
-    <t>https://www.digikey.ch/de/products/detail/abracon-llc/ASDMB-24-576MHZ-LC-T/2809941</t>
+    <t>https://www.digikey.ch/en/products/detail/kyocera-avx/KC2016Z24-5760C1KX00/11610181</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>
@@ -732,7 +732,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-12-15 19:49:32</t>
+    <t>2024-12-15 20:10:23</t>
   </si>
   <si>
     <t>KiCost® v1.1.19 + KiBot v1.8.2</t>
@@ -3085,7 +3085,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" ht="30" customHeight="1">
       <c r="A27" s="19" t="s">
         <v>105</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" ht="30" customHeight="1">
       <c r="A28" s="19" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-soundcard@69be3e94ce32679f967c18c75666e25729b23b69 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
+++ b/latest/BoM/Costs/pedalboard-soundcard-bom.xlsx
@@ -277,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="171">
   <si>
     <t>Row</t>
   </si>
@@ -309,6 +309,9 @@
     <t>Supplier</t>
   </si>
   <si>
+    <t>Sim.Pins</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -414,6 +417,9 @@
     <t>~</t>
   </si>
   <si>
+    <t>1=K 2=A</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
@@ -651,7 +657,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>8.0.6+1</t>
+    <t>9.0.1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -717,6 +723,9 @@
     <t>Film Capacitor</t>
   </si>
   <si>
+    <t>Light emitting diode</t>
+  </si>
+  <si>
     <t>250mA low-noise LDO, 2.2V-5.5V input, 3.3V output, SOT-23-5</t>
   </si>
   <si>
@@ -732,10 +741,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-12-16 18:22:56</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.19 + KiBot v1.8.2</t>
+    <t>2025-04-21 12:47:56</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.20 + KiBot v1.8.4</t>
   </si>
   <si>
     <t>Columns colors</t>
@@ -1131,10 +1140,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>957675</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>297815</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>16584</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1161,7 +1170,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9396825" cy="5079365"/>
+          <a:ext cx="2378784" cy="1285829"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1183,10 +1192,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2691225</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>107315</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>16584</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1213,7 +1222,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9396825" cy="5079365"/>
+          <a:ext cx="2378784" cy="1285829"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1235,10 +1244,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1452975</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>107315</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2378784</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1265,7 +1274,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9396825" cy="5079365"/>
+          <a:ext cx="2378784" cy="1285829"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1287,10 +1296,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1338675</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>107315</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>750009</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1317,7 +1326,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9396825" cy="5079365"/>
+          <a:ext cx="2378784" cy="1285829"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1614,7 +1623,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1633,11 +1642,12 @@
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
     <col min="10" max="10" width="60.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32" customHeight="1">
+    <row r="1" spans="1:11" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1646,78 +1656,79 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="C2" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F2" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="C3" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="C4" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="C5" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="C6" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F6" s="3">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -1748,618 +1759,678 @@
       <c r="J8" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="30" customHeight="1">
+      <c r="K8" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="30" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="30" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="30" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="45" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30" customHeight="1">
+      <c r="A16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="5" t="s">
+      <c r="H16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30" customHeight="1">
+      <c r="A17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30" customHeight="1">
+      <c r="A18" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="H18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="30" customHeight="1">
-      <c r="A10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="10" t="s">
+      <c r="I18" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" customHeight="1">
+      <c r="A20" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="45" customHeight="1">
+      <c r="A22" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="30" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="H22" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" customHeight="1">
+      <c r="A24" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="7" t="s">
+      <c r="H24" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1">
-      <c r="A12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="10" t="s">
+      <c r="I24" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="11" t="s">
+      <c r="H25" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="30" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="I25" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30" customHeight="1">
+      <c r="A26" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="7" t="s">
+      <c r="H26" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="10" t="s">
+      <c r="I26" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="45" customHeight="1">
-      <c r="A15" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1">
-      <c r="A16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="30" customHeight="1">
-      <c r="A18" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="30" customHeight="1">
-      <c r="A19" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="30" customHeight="1">
-      <c r="A20" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="30" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="45" customHeight="1">
-      <c r="A22" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="30" customHeight="1">
-      <c r="A23" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="30" customHeight="1">
-      <c r="A24" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="30" customHeight="1">
-      <c r="A25" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="30" customHeight="1">
-      <c r="A26" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="J26" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="30" customHeight="1">
-      <c r="A27" s="5" t="s">
+      <c r="H27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>108</v>
-      </c>
       <c r="J27" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -2369,7 +2440,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -2388,11 +2459,12 @@
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
     <col min="10" max="10" width="60.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32" customHeight="1">
+    <row r="1" spans="1:11" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2401,78 +2473,79 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="C2" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F2" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="C3" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="C4" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="C5" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="C6" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F6" s="3">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -2503,74 +2576,83 @@
       <c r="J8" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="30" customHeight="1">
+      <c r="K8" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="30" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="J9" s="8" t="s">
+      <c r="H10" s="9" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="30" customHeight="1">
-      <c r="A10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>136</v>
-      </c>
       <c r="I10" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -2603,7 +2685,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2612,13 +2694,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="H2" s="13">
         <v>1</v>
@@ -2626,13 +2708,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2641,13 +2723,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="H4" s="16">
         <f>SUM(H10:H28)</f>
@@ -2656,23 +2738,23 @@
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2696,30 +2778,30 @@
         <v>5</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1">
       <c r="A10" s="19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2732,19 +2814,19 @@
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1">
       <c r="A11" s="19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F11" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2757,16 +2839,16 @@
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F12" s="19">
         <f>CEILING(BoardQty*9,1)</f>
@@ -2779,16 +2861,16 @@
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1">
       <c r="A13" s="19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F13" s="19">
         <f>CEILING(BoardQty*8,1)</f>
@@ -2801,16 +2883,16 @@
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1">
       <c r="A14" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F14" s="19">
         <f>CEILING(BoardQty*11,1)</f>
@@ -2823,13 +2905,16 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>148</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2842,16 +2927,16 @@
     </row>
     <row r="16" spans="1:8" ht="45" customHeight="1">
       <c r="A16" s="19" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F16" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2864,16 +2949,16 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="19" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F17" s="19">
         <f>BoardQty*1</f>
@@ -2886,16 +2971,16 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F18" s="19">
         <f>CEILING(BoardQty*10,1)</f>
@@ -2908,16 +2993,16 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="19" t="s">
         <v>63</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>61</v>
       </c>
       <c r="F19" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2930,16 +3015,16 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F20" s="19">
         <f>CEILING(BoardQty*3,1)</f>
@@ -2952,16 +3037,16 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F21" s="19">
         <f>CEILING(BoardQty*5,1)</f>
@@ -2974,16 +3059,16 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F22" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -2996,16 +3081,16 @@
     </row>
     <row r="23" spans="1:8" ht="45" customHeight="1">
       <c r="A23" s="19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F23" s="19">
         <f>BoardQty*1</f>
@@ -3018,19 +3103,19 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="19" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F24" s="19">
         <f>CEILING(BoardQty*3,1)</f>
@@ -3043,16 +3128,16 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="19" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F25" s="19">
         <f>BoardQty*1</f>
@@ -3065,16 +3150,16 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F26" s="19">
         <f>BoardQty*1</f>
@@ -3087,16 +3172,16 @@
     </row>
     <row r="27" spans="1:8" ht="30" customHeight="1">
       <c r="A27" s="19" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F27" s="19">
         <f>BoardQty*1</f>
@@ -3109,16 +3194,16 @@
     </row>
     <row r="28" spans="1:8" ht="30" customHeight="1">
       <c r="A28" s="19" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F28" s="19">
         <f>BoardQty*1</f>
@@ -3131,15 +3216,15 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="21" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="23" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3292,7 +3377,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3300,13 +3385,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3314,13 +3399,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3329,13 +3414,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G11)</f>
@@ -3344,23 +3429,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3380,30 +3465,30 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3416,16 +3501,16 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E11" s="19">
         <f>BoardQty*1</f>
@@ -3438,15 +3523,15 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="21" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="23" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3487,77 +3572,77 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="24" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="25" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="26" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="27" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="28" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="29" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="30" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="31" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="32" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>